<commit_message>
Mysterious samples not added
</commit_message>
<xml_diff>
--- a/metadata/excel/projects/micans/micans_v6_exp1/metadata.xlsx
+++ b/metadata/excel/projects/micans/micans_v6_exp1/metadata.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="232">
   <si>
     <t>Country</t>
   </si>
@@ -814,6 +814,12 @@
   </si>
   <si>
     <t>mysterious/</t>
+  </si>
+  <si>
+    <t>Unknown barcode "TCAGC" of last pool</t>
+  </si>
+  <si>
+    <t>All mysterious samples</t>
   </si>
 </sst>
 </file>
@@ -2168,10 +2174,10 @@
   </sheetPr>
   <dimension ref="A1:CC65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="114" zoomScalePageLayoutView="114" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="114" zoomScaleNormal="114" zoomScalePageLayoutView="114" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="BC37" sqref="BC37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7235,21 +7241,76 @@
       <c r="P35" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="W35"/>
-      <c r="X35"/>
-      <c r="Z35" s="2"/>
-      <c r="AA35"/>
-      <c r="AB35"/>
-      <c r="AC35" s="2"/>
-      <c r="AD35"/>
-      <c r="AE35"/>
+      <c r="W35" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="X35" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="Z35" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA35" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB35" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC35" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD35" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE35" s="24" t="s">
+        <v>73</v>
+      </c>
       <c r="AH35"/>
       <c r="AJ35"/>
       <c r="AK35"/>
       <c r="AM35"/>
-      <c r="AN35" s="15"/>
-      <c r="AR35"/>
-      <c r="AT35"/>
+      <c r="AN35" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="AP35" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ35" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="AR35" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AS35" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT35" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AV35" t="s">
+        <v>8</v>
+      </c>
+      <c r="AW35" t="s">
+        <v>9</v>
+      </c>
+      <c r="AX35" t="s">
+        <v>10</v>
+      </c>
+      <c r="AY35" t="s">
+        <v>68</v>
+      </c>
+      <c r="AZ35" t="s">
+        <v>11</v>
+      </c>
+      <c r="BA35" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC35">
+        <v>111</v>
+      </c>
+      <c r="BD35">
+        <v>111</v>
+      </c>
       <c r="BL35"/>
       <c r="BM35"/>
       <c r="BN35"/>

</xml_diff>

<commit_message>
Fix length filter problem
</commit_message>
<xml_diff>
--- a/metadata/excel/projects/micans/micans_v6_exp1/metadata.xlsx
+++ b/metadata/excel/projects/micans/micans_v6_exp1/metadata.xlsx
@@ -327,21 +327,6 @@
     <t>OLKR57.149.152mglass (150001)</t>
   </si>
   <si>
-    <t>OLKR56.398.405mgarnets (150060_garnets)</t>
-  </si>
-  <si>
-    <t>OLKR56.398.405mglass (150060_glass)</t>
-  </si>
-  <si>
-    <t>PseudomonasFluorescence10.9 (160011_10_9)</t>
-  </si>
-  <si>
-    <t>PseudomonasFluorescence10.7 (160011_10_7)</t>
-  </si>
-  <si>
-    <t>PseudomonasFluorescence10.5 (160011_10_5)</t>
-  </si>
-  <si>
     <t>DNAxNTC (160012)</t>
   </si>
   <si>
@@ -820,6 +805,21 @@
   </si>
   <si>
     <t>All mysterious samples</t>
+  </si>
+  <si>
+    <t>OLKR56.398.405mgarnets (150060)</t>
+  </si>
+  <si>
+    <t>OLKR56.398.405mglass (150060)</t>
+  </si>
+  <si>
+    <t>PseudoFluorescence10.9 (160011)</t>
+  </si>
+  <si>
+    <t>PseudoFluorescence10.7 (160011)</t>
+  </si>
+  <si>
+    <t>PseudoFluorescence10.5 (160011)</t>
   </si>
 </sst>
 </file>
@@ -2174,10 +2174,10 @@
   </sheetPr>
   <dimension ref="A1:CC65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="114" zoomScalePageLayoutView="114" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozenSplit"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="114" zoomScaleNormal="114" zoomScalePageLayoutView="114" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="BC37" sqref="BC37"/>
+      <selection pane="bottomLeft" activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2351,7 +2351,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="54" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D2" s="54" t="s">
         <v>66</v>
@@ -2361,7 +2361,7 @@
       </c>
       <c r="F2" s="55"/>
       <c r="G2" s="54" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="H2" s="54" t="s">
         <v>61</v>
@@ -2380,13 +2380,13 @@
       </c>
       <c r="M2" s="56"/>
       <c r="N2" s="54" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="O2" s="54" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="P2" s="54" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="Q2" s="56"/>
       <c r="R2" s="57" t="s">
@@ -2549,16 +2549,16 @@
         <v>31</v>
       </c>
       <c r="BY2" s="63" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="BZ2" s="63" t="s">
         <v>41</v>
       </c>
       <c r="CA2" s="63" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="CB2" s="63" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="CC2" s="59"/>
     </row>
@@ -2571,40 +2571,40 @@
         <v>1</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G3" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H3" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I3" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J3" s="39" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="K3" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L3" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="N3" s="53" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="O3" s="39" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="P3" s="34" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="R3" s="46"/>
       <c r="S3" s="49"/>
@@ -2617,7 +2617,7 @@
         <v>83</v>
       </c>
       <c r="X3" s="20" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="Y3" s="1"/>
       <c r="Z3" s="42" t="s">
@@ -2716,40 +2716,40 @@
         <v>2</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G4" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H4" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I4" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J4" s="39" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="K4" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L4" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="N4" s="53" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="O4" s="39" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="P4" s="34" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="R4" s="46"/>
       <c r="S4" s="49"/>
@@ -2762,7 +2762,7 @@
         <v>84</v>
       </c>
       <c r="X4" s="20" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="Y4" s="1"/>
       <c r="Z4" s="42" t="s">
@@ -2861,40 +2861,40 @@
         <v>3</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G5" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H5" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I5" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J5" s="39" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="K5" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L5" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="N5" s="53" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="O5" s="39" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="P5" s="34" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="R5" s="46"/>
       <c r="S5" s="49"/>
@@ -2907,7 +2907,7 @@
         <v>85</v>
       </c>
       <c r="X5" s="20" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="Y5" s="1"/>
       <c r="Z5" s="42" t="s">
@@ -3006,40 +3006,40 @@
         <v>4</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G6" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H6" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I6" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J6" s="39" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="K6" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L6" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="N6" s="53" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="O6" s="39" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="P6" s="34" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="R6" s="46"/>
       <c r="S6" s="49"/>
@@ -3052,7 +3052,7 @@
         <v>86</v>
       </c>
       <c r="X6" s="20" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="Y6" s="1"/>
       <c r="Z6" s="42" t="s">
@@ -3151,40 +3151,40 @@
         <v>5</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G7" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H7" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I7" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J7" s="39" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K7" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L7" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="N7" s="53" t="s">
+        <v>203</v>
+      </c>
+      <c r="O7" s="39" t="s">
         <v>208</v>
       </c>
-      <c r="O7" s="39" t="s">
-        <v>213</v>
-      </c>
       <c r="P7" s="34" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="R7" s="46"/>
       <c r="S7" s="49"/>
@@ -3197,7 +3197,7 @@
         <v>87</v>
       </c>
       <c r="X7" s="20" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="Y7" s="1"/>
       <c r="Z7" s="42" t="s">
@@ -3296,40 +3296,40 @@
         <v>6</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G8" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H8" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I8" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J8" s="39" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K8" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="L8" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="N8" s="53" t="s">
+        <v>206</v>
+      </c>
+      <c r="O8" s="39" t="s">
+        <v>210</v>
+      </c>
+      <c r="P8" s="34" t="s">
         <v>171</v>
-      </c>
-      <c r="L8" s="39" t="s">
-        <v>172</v>
-      </c>
-      <c r="N8" s="53" t="s">
-        <v>211</v>
-      </c>
-      <c r="O8" s="39" t="s">
-        <v>215</v>
-      </c>
-      <c r="P8" s="34" t="s">
-        <v>176</v>
       </c>
       <c r="R8" s="46"/>
       <c r="S8" s="49"/>
@@ -3342,7 +3342,7 @@
         <v>88</v>
       </c>
       <c r="X8" s="20" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="Y8" s="1"/>
       <c r="Z8" s="42" t="s">
@@ -3441,40 +3441,40 @@
         <v>7</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G9" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H9" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I9" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J9" s="39" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="K9" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="L9" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="N9" s="53" t="s">
+        <v>203</v>
+      </c>
+      <c r="O9" s="39" t="s">
+        <v>210</v>
+      </c>
+      <c r="P9" s="34" t="s">
         <v>171</v>
-      </c>
-      <c r="L9" s="39" t="s">
-        <v>172</v>
-      </c>
-      <c r="N9" s="53" t="s">
-        <v>208</v>
-      </c>
-      <c r="O9" s="39" t="s">
-        <v>215</v>
-      </c>
-      <c r="P9" s="34" t="s">
-        <v>176</v>
       </c>
       <c r="R9" s="46"/>
       <c r="S9" s="49"/>
@@ -3487,7 +3487,7 @@
         <v>89</v>
       </c>
       <c r="X9" s="20" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="Y9" s="1"/>
       <c r="Z9" s="42" t="s">
@@ -3586,40 +3586,40 @@
         <v>8</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G10" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H10" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I10" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J10" s="39" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="K10" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="L10" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="N10" s="53" t="s">
+        <v>204</v>
+      </c>
+      <c r="O10" s="39" t="s">
+        <v>210</v>
+      </c>
+      <c r="P10" s="34" t="s">
         <v>171</v>
-      </c>
-      <c r="L10" s="39" t="s">
-        <v>172</v>
-      </c>
-      <c r="N10" s="53" t="s">
-        <v>209</v>
-      </c>
-      <c r="O10" s="39" t="s">
-        <v>215</v>
-      </c>
-      <c r="P10" s="34" t="s">
-        <v>176</v>
       </c>
       <c r="R10" s="46"/>
       <c r="S10" s="49"/>
@@ -3629,10 +3629,10 @@
         <v>49</v>
       </c>
       <c r="W10" s="20" t="s">
-        <v>90</v>
+        <v>227</v>
       </c>
       <c r="X10" s="20" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="Y10" s="1"/>
       <c r="Z10" s="42" t="s">
@@ -3731,40 +3731,40 @@
         <v>9</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G11" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H11" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I11" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J11" s="39" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="K11" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="L11" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="N11" s="53" t="s">
+        <v>205</v>
+      </c>
+      <c r="O11" s="39" t="s">
+        <v>210</v>
+      </c>
+      <c r="P11" s="34" t="s">
         <v>171</v>
-      </c>
-      <c r="L11" s="39" t="s">
-        <v>172</v>
-      </c>
-      <c r="N11" s="53" t="s">
-        <v>210</v>
-      </c>
-      <c r="O11" s="39" t="s">
-        <v>215</v>
-      </c>
-      <c r="P11" s="34" t="s">
-        <v>176</v>
       </c>
       <c r="R11" s="46"/>
       <c r="S11" s="49"/>
@@ -3774,10 +3774,10 @@
         <v>49</v>
       </c>
       <c r="W11" s="20" t="s">
-        <v>91</v>
+        <v>228</v>
       </c>
       <c r="X11" s="20" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="Y11" s="1"/>
       <c r="Z11" s="42" t="s">
@@ -3876,40 +3876,40 @@
         <v>10</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G12" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H12" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I12" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J12" s="39" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="K12" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L12" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="N12" s="53" t="s">
+        <v>206</v>
+      </c>
+      <c r="O12" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="P12" s="34" t="s">
         <v>172</v>
-      </c>
-      <c r="N12" s="53" t="s">
-        <v>211</v>
-      </c>
-      <c r="O12" s="39" t="s">
-        <v>216</v>
-      </c>
-      <c r="P12" s="34" t="s">
-        <v>177</v>
       </c>
       <c r="R12" s="46"/>
       <c r="S12" s="49"/>
@@ -3919,10 +3919,10 @@
         <v>49</v>
       </c>
       <c r="W12" s="20" t="s">
-        <v>92</v>
+        <v>229</v>
       </c>
       <c r="X12" s="20" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="Y12" s="1"/>
       <c r="Z12" s="42" t="s">
@@ -4021,40 +4021,40 @@
         <v>11</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G13" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H13" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I13" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J13" s="39" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="K13" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L13" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="N13" s="53" t="s">
+        <v>207</v>
+      </c>
+      <c r="O13" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="P13" s="34" t="s">
         <v>172</v>
-      </c>
-      <c r="N13" s="53" t="s">
-        <v>212</v>
-      </c>
-      <c r="O13" s="39" t="s">
-        <v>216</v>
-      </c>
-      <c r="P13" s="34" t="s">
-        <v>177</v>
       </c>
       <c r="R13" s="46"/>
       <c r="S13" s="49"/>
@@ -4064,10 +4064,10 @@
         <v>49</v>
       </c>
       <c r="W13" s="20" t="s">
-        <v>93</v>
+        <v>230</v>
       </c>
       <c r="X13" s="20" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="Y13" s="1"/>
       <c r="Z13" s="42" t="s">
@@ -4166,40 +4166,40 @@
         <v>12</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G14" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H14" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I14" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J14" s="39" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="K14" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L14" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="N14" s="53" t="s">
+        <v>203</v>
+      </c>
+      <c r="O14" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="P14" s="34" t="s">
         <v>172</v>
-      </c>
-      <c r="N14" s="53" t="s">
-        <v>208</v>
-      </c>
-      <c r="O14" s="39" t="s">
-        <v>216</v>
-      </c>
-      <c r="P14" s="34" t="s">
-        <v>177</v>
       </c>
       <c r="R14" s="46"/>
       <c r="S14" s="49"/>
@@ -4209,10 +4209,10 @@
         <v>49</v>
       </c>
       <c r="W14" s="20" t="s">
-        <v>94</v>
+        <v>231</v>
       </c>
       <c r="X14" s="20" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="Y14" s="1"/>
       <c r="Z14" s="42" t="s">
@@ -4311,40 +4311,40 @@
         <v>13</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G15" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H15" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I15" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J15" s="39" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="K15" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L15" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="N15" s="53" t="s">
+        <v>205</v>
+      </c>
+      <c r="O15" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="P15" s="34" t="s">
         <v>172</v>
-      </c>
-      <c r="N15" s="53" t="s">
-        <v>210</v>
-      </c>
-      <c r="O15" s="39" t="s">
-        <v>216</v>
-      </c>
-      <c r="P15" s="34" t="s">
-        <v>177</v>
       </c>
       <c r="R15" s="46"/>
       <c r="S15" s="49"/>
@@ -4354,10 +4354,10 @@
         <v>49</v>
       </c>
       <c r="W15" s="20" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="X15" s="20" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="Y15" s="1"/>
       <c r="Z15" s="42" t="s">
@@ -4456,40 +4456,40 @@
         <v>14</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G16" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H16" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I16" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J16" s="39" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="K16" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L16" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="N16" s="53" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="O16" s="39" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="P16" s="34" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="R16" s="46"/>
       <c r="S16" s="49"/>
@@ -4499,10 +4499,10 @@
         <v>49</v>
       </c>
       <c r="W16" s="20" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="X16" s="20" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="Y16" s="1"/>
       <c r="Z16" s="42" t="s">
@@ -4601,40 +4601,40 @@
         <v>15</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G17" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H17" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I17" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J17" s="39" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="K17" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L17" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="N17" s="53" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="O17" s="39" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="P17" s="34" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="R17" s="46"/>
       <c r="S17" s="49"/>
@@ -4644,10 +4644,10 @@
         <v>49</v>
       </c>
       <c r="W17" s="20" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="X17" s="20" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="Y17" s="1"/>
       <c r="Z17" s="42" t="s">
@@ -4746,40 +4746,40 @@
         <v>16</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G18" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H18" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I18" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J18" s="39" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="K18" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L18" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="N18" s="53" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="O18" s="39" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="P18" s="34" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="R18" s="46"/>
       <c r="S18" s="49"/>
@@ -4789,10 +4789,10 @@
         <v>49</v>
       </c>
       <c r="W18" s="20" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="X18" s="20" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="Y18" s="1"/>
       <c r="Z18" s="42" t="s">
@@ -4891,40 +4891,40 @@
         <v>17</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G19" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H19" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I19" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J19" s="39" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="K19" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L19" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="N19" s="53" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="O19" s="39" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="P19" s="34" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="R19" s="46"/>
       <c r="S19" s="49"/>
@@ -4934,10 +4934,10 @@
         <v>49</v>
       </c>
       <c r="W19" s="20" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="X19" s="20" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="Y19" s="1"/>
       <c r="Z19" s="42" t="s">
@@ -5036,40 +5036,40 @@
         <v>18</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G20" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H20" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I20" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J20" s="39" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="K20" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L20" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="N20" s="53" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="O20" s="39" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="P20" s="34" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="R20" s="46"/>
       <c r="S20" s="49"/>
@@ -5079,10 +5079,10 @@
         <v>49</v>
       </c>
       <c r="W20" s="20" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="X20" s="20" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="Y20" s="1"/>
       <c r="Z20" s="42" t="s">
@@ -5181,40 +5181,40 @@
         <v>19</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G21" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H21" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I21" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J21" s="39" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="K21" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L21" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="N21" s="53" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="O21" s="39" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="P21" s="34" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="R21" s="46"/>
       <c r="S21" s="49"/>
@@ -5224,10 +5224,10 @@
         <v>49</v>
       </c>
       <c r="W21" s="20" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="X21" s="20" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="Y21" s="1"/>
       <c r="Z21" s="42" t="s">
@@ -5326,40 +5326,40 @@
         <v>20</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G22" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H22" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I22" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J22" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K22" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L22" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="N22" s="53" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="O22" s="39" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="P22" s="34" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="R22" s="46"/>
       <c r="S22" s="49"/>
@@ -5369,10 +5369,10 @@
         <v>49</v>
       </c>
       <c r="W22" s="20" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="X22" s="20" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="Y22" s="1"/>
       <c r="Z22" s="42" t="s">
@@ -5471,40 +5471,40 @@
         <v>21</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D23" s="34" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G23" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H23" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I23" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J23" s="39" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="K23" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L23" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="N23" s="53" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="O23" s="39" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="P23" s="34" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="R23" s="46"/>
       <c r="S23" s="49"/>
@@ -5514,10 +5514,10 @@
         <v>49</v>
       </c>
       <c r="W23" s="20" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="X23" s="20" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="Y23" s="1"/>
       <c r="Z23" s="42" t="s">
@@ -5616,34 +5616,34 @@
         <v>22</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G24" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H24" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I24" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J24" s="39" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="K24" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L24" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="N24" s="53" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="R24" s="46"/>
       <c r="S24" s="49"/>
@@ -5653,10 +5653,10 @@
         <v>49</v>
       </c>
       <c r="W24" s="20" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="X24" s="20" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="Y24" s="1"/>
       <c r="Z24" s="42" t="s">
@@ -5755,40 +5755,40 @@
         <v>23</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G25" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H25" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I25" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J25" s="39" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="K25" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L25" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="N25" s="53" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="O25" s="39" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="P25" s="34" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="R25" s="46"/>
       <c r="S25" s="49"/>
@@ -5798,10 +5798,10 @@
         <v>49</v>
       </c>
       <c r="W25" s="20" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="X25" s="20" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="Y25" s="1"/>
       <c r="Z25" s="42" t="s">
@@ -5900,40 +5900,40 @@
         <v>24</v>
       </c>
       <c r="C26" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D26" s="34" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G26" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H26" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I26" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J26" s="39" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="K26" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L26" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="N26" s="53" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="O26" s="39" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="P26" s="34" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="R26" s="46"/>
       <c r="S26" s="49"/>
@@ -5943,10 +5943,10 @@
         <v>49</v>
       </c>
       <c r="W26" s="20" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="X26" s="20" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="Y26" s="1"/>
       <c r="Z26" s="42" t="s">
@@ -6045,40 +6045,40 @@
         <v>25</v>
       </c>
       <c r="C27" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D27" s="34" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G27" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H27" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I27" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J27" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K27" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L27" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="N27" s="53" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="O27" s="39" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="P27" s="34" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="R27" s="46"/>
       <c r="S27" s="49"/>
@@ -6088,10 +6088,10 @@
         <v>49</v>
       </c>
       <c r="W27" s="20" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="X27" s="20" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="Y27" s="1"/>
       <c r="Z27" s="42" t="s">
@@ -6190,40 +6190,40 @@
         <v>26</v>
       </c>
       <c r="C28" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D28" s="34" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G28" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H28" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I28" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J28" s="39" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="K28" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L28" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="N28" s="65" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="O28" s="39" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="P28" s="34" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="R28" s="46"/>
       <c r="S28" s="49"/>
@@ -6233,10 +6233,10 @@
         <v>49</v>
       </c>
       <c r="W28" s="20" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="X28" s="20" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="Y28" s="1"/>
       <c r="Z28" s="42" t="s">
@@ -6335,40 +6335,40 @@
         <v>27</v>
       </c>
       <c r="C29" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D29" s="34" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="G29" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H29" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I29" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J29" s="39" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="K29" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L29" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="N29" s="53" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="O29" s="39" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="P29" s="34" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="R29" s="46"/>
       <c r="S29" s="49"/>
@@ -6378,10 +6378,10 @@
         <v>49</v>
       </c>
       <c r="W29" s="20" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="X29" s="20" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="Y29" s="1"/>
       <c r="Z29" s="42" t="s">
@@ -6480,40 +6480,40 @@
         <v>28</v>
       </c>
       <c r="C30" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D30" s="34" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="G30" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H30" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I30" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J30" s="39" t="s">
+        <v>161</v>
+      </c>
+      <c r="K30" s="39" t="s">
         <v>166</v>
       </c>
-      <c r="K30" s="39" t="s">
-        <v>171</v>
-      </c>
       <c r="L30" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="N30" s="53" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="O30" s="39" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="P30" s="34" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="R30" s="46"/>
       <c r="S30" s="49"/>
@@ -6523,10 +6523,10 @@
         <v>49</v>
       </c>
       <c r="W30" s="20" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="X30" s="20" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Y30" s="1"/>
       <c r="Z30" s="42" t="s">
@@ -6625,40 +6625,40 @@
         <v>29</v>
       </c>
       <c r="C31" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D31" s="34" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="G31" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H31" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I31" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J31" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="K31" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="L31" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="K31" s="39" t="s">
-        <v>171</v>
-      </c>
-      <c r="L31" s="39" t="s">
-        <v>172</v>
-      </c>
       <c r="N31" s="53" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="O31" s="39" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="P31" s="34" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="R31" s="46"/>
       <c r="S31" s="49"/>
@@ -6668,10 +6668,10 @@
         <v>49</v>
       </c>
       <c r="W31" s="20" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="X31" s="20" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Y31" s="1"/>
       <c r="Z31" s="42" t="s">
@@ -6770,40 +6770,40 @@
         <v>30</v>
       </c>
       <c r="C32" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D32" s="34" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="G32" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H32" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I32" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J32" s="39" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="K32" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L32" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="N32" s="53" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="O32" s="39" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="P32" s="34" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="R32" s="46"/>
       <c r="S32" s="49"/>
@@ -6813,10 +6813,10 @@
         <v>49</v>
       </c>
       <c r="W32" s="20" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="X32" s="20" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Y32" s="1"/>
       <c r="Z32" s="42" t="s">
@@ -6915,40 +6915,40 @@
         <v>31</v>
       </c>
       <c r="C33" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D33" s="34" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="G33" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H33" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I33" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J33" s="39" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="K33" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L33" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="N33" s="53" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="O33" s="39" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="P33" s="34" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="R33" s="46"/>
       <c r="S33" s="49"/>
@@ -6958,10 +6958,10 @@
         <v>49</v>
       </c>
       <c r="W33" s="20" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="X33" s="20" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Y33" s="1"/>
       <c r="Z33" s="42" t="s">
@@ -7060,40 +7060,40 @@
         <v>32</v>
       </c>
       <c r="C34" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="G34" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H34" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I34" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J34" s="39" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K34" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L34" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="N34" s="53" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="O34" s="39" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="P34" s="34" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="R34" s="46"/>
       <c r="S34" s="49"/>
@@ -7103,10 +7103,10 @@
         <v>49</v>
       </c>
       <c r="W34" s="20" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="X34" s="20" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Y34" s="1"/>
       <c r="Z34" s="42" t="s">
@@ -7205,47 +7205,47 @@
         <v>33</v>
       </c>
       <c r="C35" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D35" s="34" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F35" s="36"/>
       <c r="G35" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H35" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I35" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J35" s="39" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="K35" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L35" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="N35" s="53" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="O35" s="39" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="P35" s="34" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="W35" s="20" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="X35" s="20" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="Z35" s="42" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
Reran most of it
</commit_message>
<xml_diff>
--- a/metadata/excel/projects/micans/micans_v6_exp1/metadata.xlsx
+++ b/metadata/excel/projects/micans/micans_v6_exp1/metadata.xlsx
@@ -16,10 +16,10 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
+    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="LS - Personal View" guid="{06B92370-743D-804F-912C-658BE37B1274}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="296">
   <si>
     <t>Country</t>
   </si>
@@ -820,6 +820,198 @@
   </si>
   <si>
     <t>PseudoFluorescence10.5 (160011)</t>
+  </si>
+  <si>
+    <t>62c8d402817ff3980dfc5685c10e999f</t>
+  </si>
+  <si>
+    <t>ab236c05d8d4941c2f86ac03622b9066</t>
+  </si>
+  <si>
+    <t>47988df9444d86d44562acf1215d1598</t>
+  </si>
+  <si>
+    <t>565ebc0424f0a7c817ddd4f7eecb7a87</t>
+  </si>
+  <si>
+    <t>7e30a0b1036429beacb862a490c617af</t>
+  </si>
+  <si>
+    <t>d8710cde254e3b6af94d2069871378c3</t>
+  </si>
+  <si>
+    <t>1d6dbaf9a3b26ee225ddb002e5578e35</t>
+  </si>
+  <si>
+    <t>adbd300f650ea153e8ed2e18df433498</t>
+  </si>
+  <si>
+    <t>b603a4789d7fc7c86723a0ad7d9c8825</t>
+  </si>
+  <si>
+    <t>0589c46741ea1531cc3fc0ffffbd1d9c</t>
+  </si>
+  <si>
+    <t>db5684e9e3c3a517dca631a492a5d99b</t>
+  </si>
+  <si>
+    <t>ac50a9599b1030df52143f63ecdb6536</t>
+  </si>
+  <si>
+    <t>e1454b18d01fa6d690f14456019cfe2b</t>
+  </si>
+  <si>
+    <t>0f01009793355d3b5b276932ca8eae44</t>
+  </si>
+  <si>
+    <t>c3ed231476f6da82336b96d1c8b608bf</t>
+  </si>
+  <si>
+    <t>02f11ee810840aaa211f45dbccde1a02</t>
+  </si>
+  <si>
+    <t>edd9f12f9313db486a99fc3d322bf450</t>
+  </si>
+  <si>
+    <t>cf640503d26aac6620e8d9673bfdb711</t>
+  </si>
+  <si>
+    <t>35b6b1d752ab730339b60362df4cba76</t>
+  </si>
+  <si>
+    <t>b9d894b2597d5137def1173f9118b4d2</t>
+  </si>
+  <si>
+    <t>a1c5da23dbc96a3fd10620b295884d59</t>
+  </si>
+  <si>
+    <t>6db812d1c5ffa57c96f222828990176b</t>
+  </si>
+  <si>
+    <t>6a109b5d461c6d447df0a0b9632d30cb</t>
+  </si>
+  <si>
+    <t>f661263abff1f4f84d274d05c58c6796</t>
+  </si>
+  <si>
+    <t>25714bdbe0704ec8d8dcf347b1c015b7</t>
+  </si>
+  <si>
+    <t>b2a26c174331ef4a560167e261cb057f</t>
+  </si>
+  <si>
+    <t>0f716ef2d01200a91ada975cdafd5a43</t>
+  </si>
+  <si>
+    <t>42a5e808b45f4e21010ce98fa81bd29a</t>
+  </si>
+  <si>
+    <t>117a40bf6020209e5d629679473d14bc</t>
+  </si>
+  <si>
+    <t>738016a2afb815429e6b7cd480103839</t>
+  </si>
+  <si>
+    <t>dfed8bb243a878a1dcdee20c59286034</t>
+  </si>
+  <si>
+    <t>b7378d60a5ce93dd086bad9907173d69</t>
+  </si>
+  <si>
+    <t>f2e7f57a222de52ec77bb72aeb5ef597</t>
+  </si>
+  <si>
+    <t>91658c10dc11db0f9271bf39d5542fe5</t>
+  </si>
+  <si>
+    <t>3d97b724847cd711481670eada943923</t>
+  </si>
+  <si>
+    <t>9a50c42c1f998cae0b1170ae3c48d618</t>
+  </si>
+  <si>
+    <t>152d110e5773ca7a9aa5d88c7465c314</t>
+  </si>
+  <si>
+    <t>1d8d7aebf9ae5b2a71defddeeb8bf792</t>
+  </si>
+  <si>
+    <t>b64239afd7ec618d91d137a9d69a3ea9</t>
+  </si>
+  <si>
+    <t>99c45f9f80ea275a48493a50e8db0e5b</t>
+  </si>
+  <si>
+    <t>06ee19dbeaf53587679bdc83acc0fdbb</t>
+  </si>
+  <si>
+    <t>600e811f2c87a4bcd2da72276ef972a2</t>
+  </si>
+  <si>
+    <t>be25ae0419c5f43dfc382d771be1fd0b</t>
+  </si>
+  <si>
+    <t>359a875a4dbac1015edec3da8cd4387b</t>
+  </si>
+  <si>
+    <t>5150ee869e79cc4f00768ef1187c504c</t>
+  </si>
+  <si>
+    <t>ad0c0415c54fd5ce67f9505a9a0fdc3c</t>
+  </si>
+  <si>
+    <t>ed66d5aac6b1c5f29d1a293797c3bf52</t>
+  </si>
+  <si>
+    <t>a41b2e40ddfa1b67b45407a64d408943</t>
+  </si>
+  <si>
+    <t>c5cf925498f6435709ca77bf431f3909</t>
+  </si>
+  <si>
+    <t>0c9e5fe82151377827e1812e7e548993</t>
+  </si>
+  <si>
+    <t>a2878fd0afc1ea43c00318ec5b0c329b</t>
+  </si>
+  <si>
+    <t>a1d3000e9ec40026c30927c19bbd4aa3</t>
+  </si>
+  <si>
+    <t>f9b5d9d2938b1d6becaf02ef33c7c7c9</t>
+  </si>
+  <si>
+    <t>aa8a9e5980f12173662f76221899b98a</t>
+  </si>
+  <si>
+    <t>0e31c40d56bd1576400f3ffd5fcf95d0</t>
+  </si>
+  <si>
+    <t>7300f6f1aa318bd409dd1db1ababfc23</t>
+  </si>
+  <si>
+    <t>1ad8716186c4b5a570eaffcfb0b8c9d5</t>
+  </si>
+  <si>
+    <t>d40fff701414f84683d485f415d0acb7</t>
+  </si>
+  <si>
+    <t>d8e1918baa50807618a8311375237876</t>
+  </si>
+  <si>
+    <t>02112130897ec6a2949d1ef9bee12c84</t>
+  </si>
+  <si>
+    <t>42c9c8575cc7eba4f3cc77e63dc612c2</t>
+  </si>
+  <si>
+    <t>e75771151821b3472de97d5a467cb204</t>
+  </si>
+  <si>
+    <t>c1a3ea291561e71c5ca963f003f5a86f</t>
+  </si>
+  <si>
+    <t>9695ada5af684d34641d7743e5e2d8b9</t>
   </si>
 </sst>
 </file>
@@ -1405,12 +1597,6 @@
     <xf numFmtId="11" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="11" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1486,10 +1672,16 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="290">
     <cellStyle name="Excel Built-in Normal" xfId="267"/>
@@ -1783,7 +1975,69 @@
     <cellStyle name="Hyperlink" xfId="288" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -2174,42 +2428,42 @@
   </sheetPr>
   <dimension ref="A1:CC65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="114" zoomScaleNormal="114" zoomScalePageLayoutView="114" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozenSplit"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="T17" sqref="T17"/>
+      <selection pane="bottomLeft" activeCell="V33" sqref="V33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="14" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" style="34" customWidth="1"/>
-    <col min="4" max="4" width="31.5" style="34" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" style="32" customWidth="1"/>
+    <col min="4" max="4" width="31.5" style="32" customWidth="1"/>
     <col min="5" max="5" width="27.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.5" style="14" customWidth="1"/>
-    <col min="7" max="7" width="15" style="39" customWidth="1"/>
-    <col min="8" max="8" width="33.1640625" style="39" customWidth="1"/>
-    <col min="9" max="9" width="27.6640625" style="40" customWidth="1"/>
-    <col min="10" max="10" width="17" style="39" customWidth="1"/>
-    <col min="11" max="11" width="20.5" style="39" customWidth="1"/>
-    <col min="12" max="12" width="22" style="39" customWidth="1"/>
+    <col min="7" max="7" width="15" style="37" customWidth="1"/>
+    <col min="8" max="8" width="33.1640625" style="37" customWidth="1"/>
+    <col min="9" max="9" width="27.6640625" style="38" customWidth="1"/>
+    <col min="10" max="10" width="17" style="37" customWidth="1"/>
+    <col min="11" max="11" width="20.5" style="37" customWidth="1"/>
+    <col min="12" max="12" width="22" style="37" customWidth="1"/>
     <col min="13" max="13" width="11.5" customWidth="1"/>
-    <col min="14" max="14" width="12.5" style="53" customWidth="1"/>
-    <col min="15" max="15" width="23.5" style="39" customWidth="1"/>
-    <col min="16" max="16" width="12.5" style="34" customWidth="1"/>
+    <col min="14" max="14" width="12.5" style="51" customWidth="1"/>
+    <col min="15" max="15" width="23.5" style="37" customWidth="1"/>
+    <col min="16" max="16" width="12.5" style="32" customWidth="1"/>
     <col min="17" max="17" width="11.5" customWidth="1"/>
-    <col min="18" max="18" width="15.83203125" style="47" customWidth="1"/>
-    <col min="19" max="19" width="14" style="50" customWidth="1"/>
+    <col min="18" max="18" width="15.83203125" style="45" customWidth="1"/>
+    <col min="19" max="19" width="14" style="48" customWidth="1"/>
     <col min="20" max="21" width="16.83203125" customWidth="1"/>
     <col min="22" max="22" width="11.5" customWidth="1"/>
     <col min="23" max="23" width="46.1640625" style="20" customWidth="1"/>
     <col min="24" max="24" width="44.33203125" style="20" customWidth="1"/>
     <col min="25" max="25" width="9.83203125" customWidth="1"/>
-    <col min="26" max="26" width="25.5" style="42" customWidth="1"/>
+    <col min="26" max="26" width="25.5" style="40" customWidth="1"/>
     <col min="27" max="27" width="20.1640625" style="20" customWidth="1"/>
     <col min="28" max="28" width="22" style="23" customWidth="1"/>
-    <col min="29" max="29" width="17.83203125" style="42" customWidth="1"/>
+    <col min="29" max="29" width="17.83203125" style="40" customWidth="1"/>
     <col min="30" max="30" width="21.5" style="20" customWidth="1"/>
     <col min="31" max="31" width="27.6640625" style="24" customWidth="1"/>
     <col min="32" max="32" width="9.83203125" customWidth="1"/>
@@ -2223,9 +2477,9 @@
     <col min="40" max="40" width="10.33203125" customWidth="1"/>
     <col min="41" max="41" width="11.5" customWidth="1"/>
     <col min="42" max="42" width="19.6640625" customWidth="1"/>
-    <col min="43" max="43" width="12.83203125" style="51" customWidth="1"/>
+    <col min="43" max="43" width="12.83203125" style="49" customWidth="1"/>
     <col min="44" max="44" width="32.83203125" style="1" customWidth="1"/>
-    <col min="45" max="45" width="13" style="51" customWidth="1"/>
+    <col min="45" max="45" width="13" style="49" customWidth="1"/>
     <col min="46" max="46" width="35.6640625" style="1" customWidth="1"/>
     <col min="47" max="47" width="10.1640625" customWidth="1"/>
     <col min="48" max="48" width="12.5" customWidth="1"/>
@@ -2267,31 +2521,31 @@
         <v>49</v>
       </c>
       <c r="B1" s="5"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
       <c r="E1" s="11"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="38"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="35"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="48"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="36"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="33"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="46"/>
       <c r="T1" s="5"/>
       <c r="U1" s="8"/>
       <c r="W1" s="8"/>
       <c r="X1" s="21"/>
-      <c r="Z1" s="41"/>
+      <c r="Z1" s="39"/>
       <c r="AA1" s="21"/>
       <c r="AB1" s="22"/>
-      <c r="AC1" s="43"/>
+      <c r="AC1" s="41"/>
       <c r="AD1" s="21"/>
       <c r="AE1" s="5"/>
-      <c r="AF1" s="35"/>
+      <c r="AF1" s="33"/>
       <c r="AG1" s="5"/>
       <c r="AH1" s="7"/>
       <c r="AI1" s="5"/>
@@ -2301,9 +2555,9 @@
       <c r="AM1" s="16"/>
       <c r="AN1" s="5"/>
       <c r="AP1" s="10"/>
-      <c r="AQ1" s="33"/>
+      <c r="AQ1" s="31"/>
       <c r="AR1" s="11"/>
-      <c r="AS1" s="33"/>
+      <c r="AS1" s="31"/>
       <c r="AT1" s="9"/>
       <c r="AV1" s="5"/>
       <c r="AW1" s="5"/>
@@ -2314,24 +2568,24 @@
       <c r="BB1" s="5"/>
       <c r="BC1" s="5"/>
       <c r="BD1" s="12"/>
-      <c r="BF1" s="66" t="s">
+      <c r="BF1" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="BG1" s="66"/>
-      <c r="BH1" s="66"/>
-      <c r="BI1" s="66"/>
-      <c r="BK1" s="66" t="s">
+      <c r="BG1" s="65"/>
+      <c r="BH1" s="65"/>
+      <c r="BI1" s="65"/>
+      <c r="BK1" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="BL1" s="66"/>
-      <c r="BM1" s="66"/>
-      <c r="BN1" s="66"/>
-      <c r="BO1" s="66"/>
-      <c r="BP1" s="66"/>
-      <c r="BR1" s="66" t="s">
+      <c r="BL1" s="65"/>
+      <c r="BM1" s="65"/>
+      <c r="BN1" s="65"/>
+      <c r="BO1" s="65"/>
+      <c r="BP1" s="65"/>
+      <c r="BR1" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="BS1" s="66"/>
+      <c r="BS1" s="65"/>
       <c r="BU1" s="10" t="s">
         <v>72</v>
       </c>
@@ -2343,224 +2597,224 @@
       <c r="CA1" s="25"/>
       <c r="CB1" s="25"/>
     </row>
-    <row r="2" spans="1:81" s="64" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="54" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="54" t="s">
+    <row r="2" spans="1:81" s="62" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="52" t="s">
         <v>200</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="D2" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="54" t="s">
+      <c r="E2" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="55"/>
-      <c r="G2" s="54" t="s">
+      <c r="F2" s="53"/>
+      <c r="G2" s="52" t="s">
         <v>217</v>
       </c>
-      <c r="H2" s="54" t="s">
+      <c r="H2" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="54" t="s">
+      <c r="I2" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="54" t="s">
+      <c r="J2" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="K2" s="54" t="s">
+      <c r="K2" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="L2" s="54" t="s">
+      <c r="L2" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="M2" s="56"/>
-      <c r="N2" s="54" t="s">
+      <c r="M2" s="54"/>
+      <c r="N2" s="52" t="s">
         <v>168</v>
       </c>
-      <c r="O2" s="54" t="s">
+      <c r="O2" s="52" t="s">
         <v>181</v>
       </c>
-      <c r="P2" s="54" t="s">
+      <c r="P2" s="52" t="s">
         <v>199</v>
       </c>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="57" t="s">
+      <c r="Q2" s="54"/>
+      <c r="R2" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="S2" s="57" t="s">
+      <c r="S2" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="T2" s="54" t="s">
+      <c r="T2" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="U2" s="54" t="s">
+      <c r="U2" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="V2" s="56"/>
-      <c r="W2" s="54" t="s">
+      <c r="V2" s="54"/>
+      <c r="W2" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="X2" s="54" t="s">
+      <c r="X2" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="Y2" s="56"/>
-      <c r="Z2" s="54" t="s">
+      <c r="Y2" s="54"/>
+      <c r="Z2" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="AA2" s="54" t="s">
+      <c r="AA2" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="AB2" s="54" t="s">
+      <c r="AB2" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="AC2" s="54" t="s">
+      <c r="AC2" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="AD2" s="54" t="s">
+      <c r="AD2" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="AE2" s="54" t="s">
+      <c r="AE2" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="AF2" s="56"/>
-      <c r="AG2" s="54" t="s">
+      <c r="AF2" s="54"/>
+      <c r="AG2" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="AH2" s="54" t="s">
+      <c r="AH2" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="AI2" s="54" t="s">
+      <c r="AI2" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="AJ2" s="54" t="s">
+      <c r="AJ2" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="AK2" s="54" t="s">
+      <c r="AK2" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="AL2" s="54" t="s">
+      <c r="AL2" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="AM2" s="58" t="s">
+      <c r="AM2" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="AN2" s="54" t="s">
+      <c r="AN2" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="AO2" s="56"/>
-      <c r="AP2" s="54" t="s">
+      <c r="AO2" s="54"/>
+      <c r="AP2" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="AQ2" s="54" t="s">
+      <c r="AQ2" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="AR2" s="54" t="s">
+      <c r="AR2" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="AS2" s="54" t="s">
+      <c r="AS2" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="AT2" s="54" t="s">
+      <c r="AT2" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="AU2" s="59"/>
-      <c r="AV2" s="54" t="s">
+      <c r="AU2" s="57"/>
+      <c r="AV2" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="AW2" s="54" t="s">
+      <c r="AW2" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="AX2" s="54" t="s">
+      <c r="AX2" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="AY2" s="54" t="s">
+      <c r="AY2" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="AZ2" s="54" t="s">
+      <c r="AZ2" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="BA2" s="54" t="s">
+      <c r="BA2" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="BB2" s="54" t="s">
+      <c r="BB2" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="BC2" s="54" t="s">
+      <c r="BC2" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="BD2" s="54" t="s">
+      <c r="BD2" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="BE2" s="59"/>
-      <c r="BF2" s="60" t="s">
+      <c r="BE2" s="57"/>
+      <c r="BF2" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="BG2" s="60" t="s">
+      <c r="BG2" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="BH2" s="60" t="s">
+      <c r="BH2" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="BI2" s="60" t="s">
+      <c r="BI2" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="BJ2" s="59"/>
-      <c r="BK2" s="61" t="s">
+      <c r="BJ2" s="57"/>
+      <c r="BK2" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="BL2" s="61" t="s">
+      <c r="BL2" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="BM2" s="61" t="s">
+      <c r="BM2" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="BN2" s="61" t="s">
+      <c r="BN2" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="BO2" s="61" t="s">
+      <c r="BO2" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="BP2" s="61" t="s">
+      <c r="BP2" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="BQ2" s="59"/>
-      <c r="BR2" s="62" t="s">
+      <c r="BQ2" s="57"/>
+      <c r="BR2" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="BS2" s="62" t="s">
+      <c r="BS2" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="BT2" s="59"/>
-      <c r="BU2" s="63" t="s">
+      <c r="BT2" s="57"/>
+      <c r="BU2" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="BV2" s="63" t="s">
+      <c r="BV2" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="BW2" s="63" t="s">
+      <c r="BW2" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="BX2" s="63" t="s">
+      <c r="BX2" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="BY2" s="63" t="s">
+      <c r="BY2" s="61" t="s">
         <v>178</v>
       </c>
-      <c r="BZ2" s="63" t="s">
+      <c r="BZ2" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="CA2" s="63" t="s">
+      <c r="CA2" s="61" t="s">
         <v>179</v>
       </c>
-      <c r="CB2" s="63" t="s">
+      <c r="CB2" s="61" t="s">
         <v>180</v>
       </c>
-      <c r="CC2" s="59"/>
+      <c r="CC2" s="57"/>
     </row>
     <row r="3" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A3" s="14">
@@ -2570,46 +2824,54 @@
       <c r="B3" s="27">
         <v>1</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="32" t="s">
         <v>121</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="G3" s="39" t="s">
+      <c r="G3" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H3" s="39" t="s">
+      <c r="H3" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I3" s="40" t="s">
+      <c r="I3" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J3" s="39" t="s">
+      <c r="J3" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="K3" s="39" t="s">
+      <c r="K3" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L3" s="39" t="s">
+      <c r="L3" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N3" s="53" t="s">
+      <c r="N3" s="51" t="s">
         <v>204</v>
       </c>
-      <c r="O3" s="39" t="s">
+      <c r="O3" s="37" t="s">
         <v>208</v>
       </c>
-      <c r="P3" s="34" t="s">
+      <c r="P3" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="R3" s="46"/>
-      <c r="S3" s="49"/>
-      <c r="T3" s="31"/>
-      <c r="U3" s="23"/>
+      <c r="R3" s="44">
+        <v>2820243</v>
+      </c>
+      <c r="S3" s="47">
+        <v>2820243</v>
+      </c>
+      <c r="T3" s="66" t="s">
+        <v>232</v>
+      </c>
+      <c r="U3" s="23" t="s">
+        <v>264</v>
+      </c>
       <c r="V3" t="s">
         <v>49</v>
       </c>
@@ -2620,7 +2882,7 @@
         <v>110</v>
       </c>
       <c r="Y3" s="1"/>
-      <c r="Z3" s="42" t="s">
+      <c r="Z3" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA3" s="20" t="s">
@@ -2629,7 +2891,7 @@
       <c r="AB3" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC3" s="42" t="s">
+      <c r="AC3" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD3" s="20" t="s">
@@ -2653,13 +2915,13 @@
       <c r="AP3" t="s">
         <v>81</v>
       </c>
-      <c r="AQ3" s="51" t="s">
+      <c r="AQ3" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS3" s="51" t="s">
+      <c r="AS3" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT3" s="1" t="s">
@@ -2715,46 +2977,54 @@
       <c r="B4" s="27">
         <v>2</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="32" t="s">
         <v>122</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="G4" s="39" t="s">
+      <c r="G4" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H4" s="39" t="s">
+      <c r="H4" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I4" s="40" t="s">
+      <c r="I4" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J4" s="39" t="s">
+      <c r="J4" s="37" t="s">
         <v>152</v>
       </c>
-      <c r="K4" s="39" t="s">
+      <c r="K4" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L4" s="39" t="s">
+      <c r="L4" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N4" s="53" t="s">
+      <c r="N4" s="51" t="s">
         <v>205</v>
       </c>
-      <c r="O4" s="39" t="s">
+      <c r="O4" s="37" t="s">
         <v>208</v>
       </c>
-      <c r="P4" s="34" t="s">
+      <c r="P4" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="R4" s="46"/>
-      <c r="S4" s="49"/>
-      <c r="T4" s="31"/>
-      <c r="U4" s="23"/>
+      <c r="R4" s="44">
+        <v>1695054</v>
+      </c>
+      <c r="S4" s="47">
+        <v>1695054</v>
+      </c>
+      <c r="T4" s="66" t="s">
+        <v>233</v>
+      </c>
+      <c r="U4" s="23" t="s">
+        <v>265</v>
+      </c>
       <c r="V4" t="s">
         <v>49</v>
       </c>
@@ -2765,7 +3035,7 @@
         <v>110</v>
       </c>
       <c r="Y4" s="1"/>
-      <c r="Z4" s="42" t="s">
+      <c r="Z4" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA4" s="20" t="s">
@@ -2774,7 +3044,7 @@
       <c r="AB4" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC4" s="42" t="s">
+      <c r="AC4" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD4" s="20" t="s">
@@ -2798,13 +3068,13 @@
       <c r="AP4" t="s">
         <v>81</v>
       </c>
-      <c r="AQ4" s="51" t="s">
+      <c r="AQ4" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR4" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS4" s="51" t="s">
+      <c r="AS4" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT4" s="1" t="s">
@@ -2860,46 +3130,54 @@
       <c r="B5" s="27">
         <v>3</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="32" t="s">
         <v>123</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="G5" s="39" t="s">
+      <c r="G5" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H5" s="39" t="s">
+      <c r="H5" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I5" s="40" t="s">
+      <c r="I5" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J5" s="39" t="s">
+      <c r="J5" s="37" t="s">
         <v>153</v>
       </c>
-      <c r="K5" s="39" t="s">
+      <c r="K5" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L5" s="39" t="s">
+      <c r="L5" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N5" s="53" t="s">
+      <c r="N5" s="51" t="s">
         <v>206</v>
       </c>
-      <c r="O5" s="39" t="s">
+      <c r="O5" s="37" t="s">
         <v>209</v>
       </c>
-      <c r="P5" s="34" t="s">
+      <c r="P5" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="R5" s="46"/>
-      <c r="S5" s="49"/>
-      <c r="T5" s="31"/>
-      <c r="U5" s="28"/>
+      <c r="R5" s="44">
+        <v>1471424</v>
+      </c>
+      <c r="S5" s="47">
+        <v>1471424</v>
+      </c>
+      <c r="T5" s="66" t="s">
+        <v>234</v>
+      </c>
+      <c r="U5" s="28" t="s">
+        <v>266</v>
+      </c>
       <c r="V5" t="s">
         <v>49</v>
       </c>
@@ -2910,7 +3188,7 @@
         <v>110</v>
       </c>
       <c r="Y5" s="1"/>
-      <c r="Z5" s="42" t="s">
+      <c r="Z5" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA5" s="20" t="s">
@@ -2919,7 +3197,7 @@
       <c r="AB5" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC5" s="42" t="s">
+      <c r="AC5" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD5" s="20" t="s">
@@ -2943,13 +3221,13 @@
       <c r="AP5" t="s">
         <v>82</v>
       </c>
-      <c r="AQ5" s="51" t="s">
+      <c r="AQ5" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR5" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS5" s="51" t="s">
+      <c r="AS5" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT5" s="1" t="s">
@@ -3005,46 +3283,54 @@
       <c r="B6" s="27">
         <v>4</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="32" t="s">
         <v>124</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="G6" s="39" t="s">
+      <c r="G6" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H6" s="39" t="s">
+      <c r="H6" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I6" s="40" t="s">
+      <c r="I6" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J6" s="39" t="s">
+      <c r="J6" s="37" t="s">
         <v>154</v>
       </c>
-      <c r="K6" s="39" t="s">
+      <c r="K6" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L6" s="39" t="s">
+      <c r="L6" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N6" s="53" t="s">
+      <c r="N6" s="51" t="s">
         <v>207</v>
       </c>
-      <c r="O6" s="39" t="s">
+      <c r="O6" s="37" t="s">
         <v>209</v>
       </c>
-      <c r="P6" s="34" t="s">
+      <c r="P6" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="R6" s="46"/>
-      <c r="S6" s="49"/>
-      <c r="T6" s="32"/>
-      <c r="U6" s="23"/>
+      <c r="R6" s="44">
+        <v>1189163</v>
+      </c>
+      <c r="S6" s="47">
+        <v>1189163</v>
+      </c>
+      <c r="T6" s="67" t="s">
+        <v>235</v>
+      </c>
+      <c r="U6" s="23" t="s">
+        <v>267</v>
+      </c>
       <c r="V6" t="s">
         <v>49</v>
       </c>
@@ -3055,7 +3341,7 @@
         <v>110</v>
       </c>
       <c r="Y6" s="1"/>
-      <c r="Z6" s="42" t="s">
+      <c r="Z6" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA6" s="20" t="s">
@@ -3064,7 +3350,7 @@
       <c r="AB6" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC6" s="42" t="s">
+      <c r="AC6" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD6" s="20" t="s">
@@ -3088,13 +3374,13 @@
       <c r="AP6" t="s">
         <v>82</v>
       </c>
-      <c r="AQ6" s="51" t="s">
+      <c r="AQ6" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR6" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS6" s="51" t="s">
+      <c r="AS6" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT6" s="1" t="s">
@@ -3150,46 +3436,54 @@
       <c r="B7" s="27">
         <v>5</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="32" t="s">
         <v>125</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="G7" s="39" t="s">
+      <c r="G7" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H7" s="39" t="s">
+      <c r="H7" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I7" s="40" t="s">
+      <c r="I7" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J7" s="39" t="s">
+      <c r="J7" s="37" t="s">
         <v>155</v>
       </c>
-      <c r="K7" s="39" t="s">
+      <c r="K7" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L7" s="39" t="s">
+      <c r="L7" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N7" s="53" t="s">
+      <c r="N7" s="51" t="s">
         <v>203</v>
       </c>
-      <c r="O7" s="39" t="s">
+      <c r="O7" s="37" t="s">
         <v>208</v>
       </c>
-      <c r="P7" s="34" t="s">
+      <c r="P7" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="R7" s="46"/>
-      <c r="S7" s="49"/>
-      <c r="T7" s="31"/>
-      <c r="U7" s="23"/>
+      <c r="R7" s="44">
+        <v>1518563</v>
+      </c>
+      <c r="S7" s="47">
+        <v>1518563</v>
+      </c>
+      <c r="T7" s="66" t="s">
+        <v>236</v>
+      </c>
+      <c r="U7" s="23" t="s">
+        <v>268</v>
+      </c>
       <c r="V7" t="s">
         <v>49</v>
       </c>
@@ -3200,7 +3494,7 @@
         <v>110</v>
       </c>
       <c r="Y7" s="1"/>
-      <c r="Z7" s="42" t="s">
+      <c r="Z7" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA7" s="20" t="s">
@@ -3209,7 +3503,7 @@
       <c r="AB7" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC7" s="42" t="s">
+      <c r="AC7" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD7" s="20" t="s">
@@ -3233,13 +3527,13 @@
       <c r="AP7" t="s">
         <v>82</v>
       </c>
-      <c r="AQ7" s="51" t="s">
+      <c r="AQ7" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR7" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS7" s="51" t="s">
+      <c r="AS7" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT7" s="1" t="s">
@@ -3295,46 +3589,54 @@
       <c r="B8" s="27">
         <v>6</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="32" t="s">
         <v>126</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G8" s="39" t="s">
+      <c r="G8" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I8" s="40" t="s">
+      <c r="I8" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J8" s="39" t="s">
+      <c r="J8" s="37" t="s">
         <v>156</v>
       </c>
-      <c r="K8" s="39" t="s">
+      <c r="K8" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L8" s="39" t="s">
+      <c r="L8" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N8" s="53" t="s">
+      <c r="N8" s="51" t="s">
         <v>206</v>
       </c>
-      <c r="O8" s="39" t="s">
+      <c r="O8" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="P8" s="34" t="s">
+      <c r="P8" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="R8" s="46"/>
-      <c r="S8" s="49"/>
-      <c r="T8" s="31"/>
-      <c r="U8" s="28"/>
+      <c r="R8" s="44">
+        <v>1992368</v>
+      </c>
+      <c r="S8" s="47">
+        <v>1992368</v>
+      </c>
+      <c r="T8" s="66" t="s">
+        <v>237</v>
+      </c>
+      <c r="U8" s="28" t="s">
+        <v>269</v>
+      </c>
       <c r="V8" t="s">
         <v>49</v>
       </c>
@@ -3345,7 +3647,7 @@
         <v>111</v>
       </c>
       <c r="Y8" s="1"/>
-      <c r="Z8" s="42" t="s">
+      <c r="Z8" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA8" s="20" t="s">
@@ -3354,7 +3656,7 @@
       <c r="AB8" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC8" s="42" t="s">
+      <c r="AC8" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD8" s="20" t="s">
@@ -3378,13 +3680,13 @@
       <c r="AP8" t="s">
         <v>82</v>
       </c>
-      <c r="AQ8" s="51" t="s">
+      <c r="AQ8" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR8" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS8" s="51" t="s">
+      <c r="AS8" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT8" s="1" t="s">
@@ -3440,46 +3742,54 @@
       <c r="B9" s="27">
         <v>7</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D9" s="32" t="s">
         <v>127</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G9" s="39" t="s">
+      <c r="G9" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H9" s="39" t="s">
+      <c r="H9" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I9" s="40" t="s">
+      <c r="I9" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J9" s="39" t="s">
+      <c r="J9" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="K9" s="39" t="s">
+      <c r="K9" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L9" s="39" t="s">
+      <c r="L9" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N9" s="53" t="s">
+      <c r="N9" s="51" t="s">
         <v>203</v>
       </c>
-      <c r="O9" s="39" t="s">
+      <c r="O9" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="P9" s="34" t="s">
+      <c r="P9" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="R9" s="46"/>
-      <c r="S9" s="49"/>
-      <c r="T9" s="31"/>
-      <c r="U9" s="23"/>
+      <c r="R9" s="44">
+        <v>778194</v>
+      </c>
+      <c r="S9" s="47">
+        <v>778194</v>
+      </c>
+      <c r="T9" s="66" t="s">
+        <v>238</v>
+      </c>
+      <c r="U9" s="23" t="s">
+        <v>270</v>
+      </c>
       <c r="V9" t="s">
         <v>49</v>
       </c>
@@ -3490,7 +3800,7 @@
         <v>111</v>
       </c>
       <c r="Y9" s="1"/>
-      <c r="Z9" s="42" t="s">
+      <c r="Z9" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA9" s="20" t="s">
@@ -3499,7 +3809,7 @@
       <c r="AB9" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC9" s="42" t="s">
+      <c r="AC9" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD9" s="20" t="s">
@@ -3523,13 +3833,13 @@
       <c r="AP9" t="s">
         <v>82</v>
       </c>
-      <c r="AQ9" s="51" t="s">
+      <c r="AQ9" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS9" s="51" t="s">
+      <c r="AS9" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT9" s="1" t="s">
@@ -3585,46 +3895,54 @@
       <c r="B10" s="27">
         <v>8</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="32" t="s">
         <v>220</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G10" s="39" t="s">
+      <c r="G10" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H10" s="39" t="s">
+      <c r="H10" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I10" s="40" t="s">
+      <c r="I10" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J10" s="39" t="s">
+      <c r="J10" s="37" t="s">
         <v>182</v>
       </c>
-      <c r="K10" s="39" t="s">
+      <c r="K10" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L10" s="39" t="s">
+      <c r="L10" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N10" s="53" t="s">
+      <c r="N10" s="51" t="s">
         <v>204</v>
       </c>
-      <c r="O10" s="39" t="s">
+      <c r="O10" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="P10" s="34" t="s">
+      <c r="P10" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="R10" s="46"/>
-      <c r="S10" s="49"/>
-      <c r="T10" s="31"/>
-      <c r="U10" s="23"/>
+      <c r="R10" s="44">
+        <v>2162643</v>
+      </c>
+      <c r="S10" s="47">
+        <v>2162643</v>
+      </c>
+      <c r="T10" s="66" t="s">
+        <v>239</v>
+      </c>
+      <c r="U10" s="23" t="s">
+        <v>271</v>
+      </c>
       <c r="V10" t="s">
         <v>49</v>
       </c>
@@ -3635,7 +3953,7 @@
         <v>111</v>
       </c>
       <c r="Y10" s="1"/>
-      <c r="Z10" s="42" t="s">
+      <c r="Z10" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA10" s="20" t="s">
@@ -3644,7 +3962,7 @@
       <c r="AB10" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC10" s="42" t="s">
+      <c r="AC10" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD10" s="20" t="s">
@@ -3668,13 +3986,13 @@
       <c r="AP10" t="s">
         <v>82</v>
       </c>
-      <c r="AQ10" s="51" t="s">
+      <c r="AQ10" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR10" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS10" s="51" t="s">
+      <c r="AS10" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT10" s="1" t="s">
@@ -3730,46 +4048,54 @@
       <c r="B11" s="27">
         <v>9</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D11" s="32" t="s">
         <v>221</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G11" s="39" t="s">
+      <c r="G11" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H11" s="39" t="s">
+      <c r="H11" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I11" s="40" t="s">
+      <c r="I11" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J11" s="39" t="s">
+      <c r="J11" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="K11" s="39" t="s">
+      <c r="K11" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L11" s="39" t="s">
+      <c r="L11" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N11" s="53" t="s">
+      <c r="N11" s="51" t="s">
         <v>205</v>
       </c>
-      <c r="O11" s="39" t="s">
+      <c r="O11" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="P11" s="34" t="s">
+      <c r="P11" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="R11" s="46"/>
-      <c r="S11" s="49"/>
-      <c r="T11" s="31"/>
-      <c r="U11" s="23"/>
+      <c r="R11" s="44">
+        <v>550318</v>
+      </c>
+      <c r="S11" s="47">
+        <v>550318</v>
+      </c>
+      <c r="T11" s="66" t="s">
+        <v>240</v>
+      </c>
+      <c r="U11" s="23" t="s">
+        <v>272</v>
+      </c>
       <c r="V11" t="s">
         <v>49</v>
       </c>
@@ -3780,7 +4106,7 @@
         <v>111</v>
       </c>
       <c r="Y11" s="1"/>
-      <c r="Z11" s="42" t="s">
+      <c r="Z11" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA11" s="20" t="s">
@@ -3789,7 +4115,7 @@
       <c r="AB11" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC11" s="42" t="s">
+      <c r="AC11" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD11" s="20" t="s">
@@ -3813,13 +4139,13 @@
       <c r="AP11" t="s">
         <v>82</v>
       </c>
-      <c r="AQ11" s="51" t="s">
+      <c r="AQ11" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR11" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS11" s="51" t="s">
+      <c r="AS11" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT11" s="1" t="s">
@@ -3875,46 +4201,54 @@
       <c r="B12" s="27">
         <v>10</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="32" t="s">
         <v>128</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="G12" s="39" t="s">
+      <c r="G12" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H12" s="39" t="s">
+      <c r="H12" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I12" s="40" t="s">
+      <c r="I12" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="39" t="s">
+      <c r="J12" s="37" t="s">
         <v>184</v>
       </c>
-      <c r="K12" s="39" t="s">
+      <c r="K12" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L12" s="39" t="s">
+      <c r="L12" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N12" s="53" t="s">
+      <c r="N12" s="51" t="s">
         <v>206</v>
       </c>
-      <c r="O12" s="39" t="s">
+      <c r="O12" s="37" t="s">
         <v>211</v>
       </c>
-      <c r="P12" s="34" t="s">
+      <c r="P12" s="32" t="s">
         <v>172</v>
       </c>
-      <c r="R12" s="46"/>
-      <c r="S12" s="49"/>
-      <c r="T12" s="31"/>
-      <c r="U12" s="23"/>
+      <c r="R12" s="44">
+        <v>1673873</v>
+      </c>
+      <c r="S12" s="47">
+        <v>1673873</v>
+      </c>
+      <c r="T12" s="66" t="s">
+        <v>241</v>
+      </c>
+      <c r="U12" s="28" t="s">
+        <v>273</v>
+      </c>
       <c r="V12" t="s">
         <v>49</v>
       </c>
@@ -3925,7 +4259,7 @@
         <v>112</v>
       </c>
       <c r="Y12" s="1"/>
-      <c r="Z12" s="42" t="s">
+      <c r="Z12" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA12" s="20" t="s">
@@ -3934,7 +4268,7 @@
       <c r="AB12" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC12" s="42" t="s">
+      <c r="AC12" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD12" s="20" t="s">
@@ -3958,13 +4292,13 @@
       <c r="AP12" t="s">
         <v>82</v>
       </c>
-      <c r="AQ12" s="51" t="s">
+      <c r="AQ12" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR12" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS12" s="51" t="s">
+      <c r="AS12" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT12" s="1" t="s">
@@ -4020,46 +4354,54 @@
       <c r="B13" s="27">
         <v>11</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D13" s="34" t="s">
+      <c r="D13" s="32" t="s">
         <v>129</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="G13" s="39" t="s">
+      <c r="G13" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H13" s="39" t="s">
+      <c r="H13" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I13" s="40" t="s">
+      <c r="I13" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J13" s="39" t="s">
+      <c r="J13" s="37" t="s">
         <v>185</v>
       </c>
-      <c r="K13" s="39" t="s">
+      <c r="K13" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L13" s="39" t="s">
+      <c r="L13" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N13" s="53" t="s">
+      <c r="N13" s="51" t="s">
         <v>207</v>
       </c>
-      <c r="O13" s="39" t="s">
+      <c r="O13" s="37" t="s">
         <v>211</v>
       </c>
-      <c r="P13" s="34" t="s">
+      <c r="P13" s="32" t="s">
         <v>172</v>
       </c>
-      <c r="R13" s="46"/>
-      <c r="S13" s="49"/>
-      <c r="T13" s="31"/>
-      <c r="U13" s="23"/>
+      <c r="R13" s="44">
+        <v>1249513</v>
+      </c>
+      <c r="S13" s="47">
+        <v>1249513</v>
+      </c>
+      <c r="T13" s="66" t="s">
+        <v>242</v>
+      </c>
+      <c r="U13" s="23" t="s">
+        <v>274</v>
+      </c>
       <c r="V13" t="s">
         <v>49</v>
       </c>
@@ -4070,7 +4412,7 @@
         <v>112</v>
       </c>
       <c r="Y13" s="1"/>
-      <c r="Z13" s="42" t="s">
+      <c r="Z13" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA13" s="20" t="s">
@@ -4079,7 +4421,7 @@
       <c r="AB13" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC13" s="42" t="s">
+      <c r="AC13" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD13" s="20" t="s">
@@ -4103,13 +4445,13 @@
       <c r="AP13" t="s">
         <v>82</v>
       </c>
-      <c r="AQ13" s="51" t="s">
+      <c r="AQ13" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR13" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS13" s="51" t="s">
+      <c r="AS13" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT13" s="1" t="s">
@@ -4165,46 +4507,54 @@
       <c r="B14" s="27">
         <v>12</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="D14" s="32" t="s">
         <v>130</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="G14" s="39" t="s">
+      <c r="G14" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H14" s="39" t="s">
+      <c r="H14" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I14" s="40" t="s">
+      <c r="I14" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J14" s="39" t="s">
+      <c r="J14" s="37" t="s">
         <v>186</v>
       </c>
-      <c r="K14" s="39" t="s">
+      <c r="K14" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L14" s="39" t="s">
+      <c r="L14" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N14" s="53" t="s">
+      <c r="N14" s="51" t="s">
         <v>203</v>
       </c>
-      <c r="O14" s="39" t="s">
+      <c r="O14" s="37" t="s">
         <v>211</v>
       </c>
-      <c r="P14" s="34" t="s">
+      <c r="P14" s="32" t="s">
         <v>172</v>
       </c>
-      <c r="R14" s="46"/>
-      <c r="S14" s="49"/>
-      <c r="T14" s="31"/>
-      <c r="U14" s="23"/>
+      <c r="R14" s="44">
+        <v>629046</v>
+      </c>
+      <c r="S14" s="47">
+        <v>629046</v>
+      </c>
+      <c r="T14" s="66" t="s">
+        <v>243</v>
+      </c>
+      <c r="U14" s="23" t="s">
+        <v>275</v>
+      </c>
       <c r="V14" t="s">
         <v>49</v>
       </c>
@@ -4215,7 +4565,7 @@
         <v>112</v>
       </c>
       <c r="Y14" s="1"/>
-      <c r="Z14" s="42" t="s">
+      <c r="Z14" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA14" s="20" t="s">
@@ -4224,7 +4574,7 @@
       <c r="AB14" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC14" s="42" t="s">
+      <c r="AC14" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD14" s="20" t="s">
@@ -4248,13 +4598,13 @@
       <c r="AP14" t="s">
         <v>82</v>
       </c>
-      <c r="AQ14" s="51" t="s">
+      <c r="AQ14" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR14" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS14" s="51" t="s">
+      <c r="AS14" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT14" s="1" t="s">
@@ -4310,46 +4660,54 @@
       <c r="B15" s="27">
         <v>13</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="32" t="s">
         <v>131</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="G15" s="39" t="s">
+      <c r="G15" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H15" s="39" t="s">
+      <c r="H15" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I15" s="40" t="s">
+      <c r="I15" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J15" s="39" t="s">
+      <c r="J15" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="K15" s="39" t="s">
+      <c r="K15" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L15" s="39" t="s">
+      <c r="L15" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N15" s="53" t="s">
+      <c r="N15" s="51" t="s">
         <v>205</v>
       </c>
-      <c r="O15" s="39" t="s">
+      <c r="O15" s="37" t="s">
         <v>211</v>
       </c>
-      <c r="P15" s="34" t="s">
+      <c r="P15" s="32" t="s">
         <v>172</v>
       </c>
-      <c r="R15" s="46"/>
-      <c r="S15" s="49"/>
-      <c r="T15" s="31"/>
-      <c r="U15" s="23"/>
+      <c r="R15" s="44">
+        <v>96651</v>
+      </c>
+      <c r="S15" s="47">
+        <v>96651</v>
+      </c>
+      <c r="T15" s="66" t="s">
+        <v>244</v>
+      </c>
+      <c r="U15" s="23" t="s">
+        <v>276</v>
+      </c>
       <c r="V15" t="s">
         <v>49</v>
       </c>
@@ -4360,7 +4718,7 @@
         <v>112</v>
       </c>
       <c r="Y15" s="1"/>
-      <c r="Z15" s="42" t="s">
+      <c r="Z15" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA15" s="20" t="s">
@@ -4369,7 +4727,7 @@
       <c r="AB15" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC15" s="42" t="s">
+      <c r="AC15" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD15" s="20" t="s">
@@ -4393,13 +4751,13 @@
       <c r="AP15" t="s">
         <v>82</v>
       </c>
-      <c r="AQ15" s="51" t="s">
+      <c r="AQ15" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR15" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS15" s="51" t="s">
+      <c r="AS15" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT15" s="1" t="s">
@@ -4455,46 +4813,54 @@
       <c r="B16" s="27">
         <v>14</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="32" t="s">
         <v>132</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="G16" s="39" t="s">
+      <c r="G16" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H16" s="39" t="s">
+      <c r="H16" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I16" s="40" t="s">
+      <c r="I16" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J16" s="39" t="s">
+      <c r="J16" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="K16" s="39" t="s">
+      <c r="K16" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L16" s="39" t="s">
+      <c r="L16" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N16" s="53" t="s">
+      <c r="N16" s="51" t="s">
         <v>206</v>
       </c>
-      <c r="O16" s="39" t="s">
+      <c r="O16" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="P16" s="34" t="s">
+      <c r="P16" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="R16" s="46"/>
-      <c r="S16" s="49"/>
-      <c r="T16" s="31"/>
-      <c r="U16" s="23"/>
+      <c r="R16" s="44">
+        <v>173299</v>
+      </c>
+      <c r="S16" s="47">
+        <v>173299</v>
+      </c>
+      <c r="T16" s="66" t="s">
+        <v>245</v>
+      </c>
+      <c r="U16" s="23" t="s">
+        <v>277</v>
+      </c>
       <c r="V16" t="s">
         <v>49</v>
       </c>
@@ -4505,7 +4871,7 @@
         <v>112</v>
       </c>
       <c r="Y16" s="1"/>
-      <c r="Z16" s="42" t="s">
+      <c r="Z16" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA16" s="20" t="s">
@@ -4514,7 +4880,7 @@
       <c r="AB16" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC16" s="42" t="s">
+      <c r="AC16" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD16" s="20" t="s">
@@ -4538,13 +4904,13 @@
       <c r="AP16" t="s">
         <v>82</v>
       </c>
-      <c r="AQ16" s="51" t="s">
+      <c r="AQ16" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR16" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS16" s="51" t="s">
+      <c r="AS16" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT16" s="1" t="s">
@@ -4600,46 +4966,54 @@
       <c r="B17" s="27">
         <v>15</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="D17" s="32" t="s">
         <v>133</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G17" s="39" t="s">
+      <c r="G17" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H17" s="39" t="s">
+      <c r="H17" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I17" s="40" t="s">
+      <c r="I17" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J17" s="39" t="s">
+      <c r="J17" s="37" t="s">
         <v>187</v>
       </c>
-      <c r="K17" s="39" t="s">
+      <c r="K17" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L17" s="39" t="s">
+      <c r="L17" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N17" s="53" t="s">
+      <c r="N17" s="51" t="s">
         <v>204</v>
       </c>
-      <c r="O17" s="39" t="s">
+      <c r="O17" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="P17" s="34" t="s">
+      <c r="P17" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="R17" s="46"/>
-      <c r="S17" s="49"/>
-      <c r="T17" s="32"/>
-      <c r="U17" s="23"/>
+      <c r="R17" s="44">
+        <v>1867219</v>
+      </c>
+      <c r="S17" s="47">
+        <v>1867219</v>
+      </c>
+      <c r="T17" s="67" t="s">
+        <v>246</v>
+      </c>
+      <c r="U17" s="23" t="s">
+        <v>278</v>
+      </c>
       <c r="V17" t="s">
         <v>49</v>
       </c>
@@ -4650,7 +5024,7 @@
         <v>113</v>
       </c>
       <c r="Y17" s="1"/>
-      <c r="Z17" s="42" t="s">
+      <c r="Z17" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA17" s="20" t="s">
@@ -4659,7 +5033,7 @@
       <c r="AB17" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC17" s="42" t="s">
+      <c r="AC17" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD17" s="20" t="s">
@@ -4683,13 +5057,13 @@
       <c r="AP17" t="s">
         <v>82</v>
       </c>
-      <c r="AQ17" s="51" t="s">
+      <c r="AQ17" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR17" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS17" s="51" t="s">
+      <c r="AS17" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT17" s="1" t="s">
@@ -4745,46 +5119,54 @@
       <c r="B18" s="27">
         <v>16</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D18" s="32" t="s">
         <v>134</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G18" s="39" t="s">
+      <c r="G18" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H18" s="39" t="s">
+      <c r="H18" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I18" s="40" t="s">
+      <c r="I18" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J18" s="39" t="s">
+      <c r="J18" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="K18" s="39" t="s">
+      <c r="K18" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L18" s="39" t="s">
+      <c r="L18" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N18" s="53" t="s">
+      <c r="N18" s="51" t="s">
         <v>205</v>
       </c>
-      <c r="O18" s="39" t="s">
+      <c r="O18" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="P18" s="34" t="s">
+      <c r="P18" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="R18" s="46"/>
-      <c r="S18" s="49"/>
-      <c r="T18" s="31"/>
-      <c r="U18" s="23"/>
+      <c r="R18" s="44">
+        <v>1495186</v>
+      </c>
+      <c r="S18" s="47">
+        <v>1495186</v>
+      </c>
+      <c r="T18" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="U18" s="23" t="s">
+        <v>279</v>
+      </c>
       <c r="V18" t="s">
         <v>49</v>
       </c>
@@ -4795,7 +5177,7 @@
         <v>113</v>
       </c>
       <c r="Y18" s="1"/>
-      <c r="Z18" s="42" t="s">
+      <c r="Z18" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA18" s="20" t="s">
@@ -4804,7 +5186,7 @@
       <c r="AB18" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC18" s="42" t="s">
+      <c r="AC18" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD18" s="20" t="s">
@@ -4828,13 +5210,13 @@
       <c r="AP18" t="s">
         <v>82</v>
       </c>
-      <c r="AQ18" s="51" t="s">
+      <c r="AQ18" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR18" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS18" s="51" t="s">
+      <c r="AS18" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT18" s="1" t="s">
@@ -4890,46 +5272,54 @@
       <c r="B19" s="27">
         <v>17</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D19" s="32" t="s">
         <v>135</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G19" s="39" t="s">
+      <c r="G19" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H19" s="39" t="s">
+      <c r="H19" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I19" s="40" t="s">
+      <c r="I19" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J19" s="39" t="s">
+      <c r="J19" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="K19" s="39" t="s">
+      <c r="K19" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L19" s="39" t="s">
+      <c r="L19" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N19" s="53" t="s">
+      <c r="N19" s="51" t="s">
         <v>206</v>
       </c>
-      <c r="O19" s="39" t="s">
+      <c r="O19" s="37" t="s">
         <v>213</v>
       </c>
-      <c r="P19" s="34" t="s">
+      <c r="P19" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="R19" s="46"/>
-      <c r="S19" s="49"/>
-      <c r="T19" s="31"/>
-      <c r="U19" s="23"/>
+      <c r="R19" s="44">
+        <v>1807248</v>
+      </c>
+      <c r="S19" s="47">
+        <v>1807248</v>
+      </c>
+      <c r="T19" s="66" t="s">
+        <v>248</v>
+      </c>
+      <c r="U19" s="23" t="s">
+        <v>280</v>
+      </c>
       <c r="V19" t="s">
         <v>49</v>
       </c>
@@ -4940,7 +5330,7 @@
         <v>113</v>
       </c>
       <c r="Y19" s="1"/>
-      <c r="Z19" s="42" t="s">
+      <c r="Z19" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA19" s="20" t="s">
@@ -4949,7 +5339,7 @@
       <c r="AB19" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC19" s="42" t="s">
+      <c r="AC19" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD19" s="20" t="s">
@@ -4973,13 +5363,13 @@
       <c r="AP19" t="s">
         <v>82</v>
       </c>
-      <c r="AQ19" s="51" t="s">
+      <c r="AQ19" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR19" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS19" s="51" t="s">
+      <c r="AS19" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT19" s="1" t="s">
@@ -5035,46 +5425,54 @@
       <c r="B20" s="27">
         <v>18</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="D20" s="32" t="s">
         <v>136</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G20" s="39" t="s">
+      <c r="G20" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H20" s="39" t="s">
+      <c r="H20" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I20" s="40" t="s">
+      <c r="I20" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J20" s="39" t="s">
+      <c r="J20" s="37" t="s">
         <v>190</v>
       </c>
-      <c r="K20" s="39" t="s">
+      <c r="K20" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L20" s="39" t="s">
+      <c r="L20" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N20" s="53" t="s">
+      <c r="N20" s="51" t="s">
         <v>207</v>
       </c>
-      <c r="O20" s="39" t="s">
+      <c r="O20" s="37" t="s">
         <v>213</v>
       </c>
-      <c r="P20" s="34" t="s">
+      <c r="P20" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="R20" s="46"/>
-      <c r="S20" s="49"/>
-      <c r="T20" s="31"/>
-      <c r="U20" s="23"/>
+      <c r="R20" s="44">
+        <v>1408298</v>
+      </c>
+      <c r="S20" s="47">
+        <v>1408298</v>
+      </c>
+      <c r="T20" s="66" t="s">
+        <v>249</v>
+      </c>
+      <c r="U20" s="23" t="s">
+        <v>281</v>
+      </c>
       <c r="V20" t="s">
         <v>49</v>
       </c>
@@ -5085,7 +5483,7 @@
         <v>113</v>
       </c>
       <c r="Y20" s="1"/>
-      <c r="Z20" s="42" t="s">
+      <c r="Z20" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA20" s="20" t="s">
@@ -5094,7 +5492,7 @@
       <c r="AB20" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC20" s="42" t="s">
+      <c r="AC20" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD20" s="20" t="s">
@@ -5118,13 +5516,13 @@
       <c r="AP20" t="s">
         <v>82</v>
       </c>
-      <c r="AQ20" s="51" t="s">
+      <c r="AQ20" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR20" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS20" s="51" t="s">
+      <c r="AS20" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT20" s="1" t="s">
@@ -5180,46 +5578,54 @@
       <c r="B21" s="27">
         <v>19</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="C21" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D21" s="34" t="s">
+      <c r="D21" s="32" t="s">
         <v>137</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G21" s="39" t="s">
+      <c r="G21" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H21" s="39" t="s">
+      <c r="H21" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I21" s="40" t="s">
+      <c r="I21" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J21" s="39" t="s">
+      <c r="J21" s="37" t="s">
         <v>191</v>
       </c>
-      <c r="K21" s="39" t="s">
+      <c r="K21" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L21" s="39" t="s">
+      <c r="L21" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N21" s="53" t="s">
+      <c r="N21" s="51" t="s">
         <v>203</v>
       </c>
-      <c r="O21" s="39" t="s">
+      <c r="O21" s="37" t="s">
         <v>213</v>
       </c>
-      <c r="P21" s="34" t="s">
+      <c r="P21" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="R21" s="46"/>
-      <c r="S21" s="49"/>
-      <c r="T21" s="31"/>
-      <c r="U21" s="23"/>
+      <c r="R21" s="44">
+        <v>3202907</v>
+      </c>
+      <c r="S21" s="47">
+        <v>3202907</v>
+      </c>
+      <c r="T21" s="66" t="s">
+        <v>250</v>
+      </c>
+      <c r="U21" s="23" t="s">
+        <v>282</v>
+      </c>
       <c r="V21" t="s">
         <v>49</v>
       </c>
@@ -5230,7 +5636,7 @@
         <v>113</v>
       </c>
       <c r="Y21" s="1"/>
-      <c r="Z21" s="42" t="s">
+      <c r="Z21" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA21" s="20" t="s">
@@ -5239,7 +5645,7 @@
       <c r="AB21" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC21" s="42" t="s">
+      <c r="AC21" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD21" s="20" t="s">
@@ -5263,13 +5669,13 @@
       <c r="AP21" t="s">
         <v>82</v>
       </c>
-      <c r="AQ21" s="51" t="s">
+      <c r="AQ21" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR21" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS21" s="51" t="s">
+      <c r="AS21" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT21" s="1" t="s">
@@ -5325,46 +5731,54 @@
       <c r="B22" s="27">
         <v>20</v>
       </c>
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="32" t="s">
         <v>138</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G22" s="39" t="s">
+      <c r="G22" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H22" s="39" t="s">
+      <c r="H22" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I22" s="40" t="s">
+      <c r="I22" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J22" s="39" t="s">
+      <c r="J22" s="37" t="s">
         <v>192</v>
       </c>
-      <c r="K22" s="39" t="s">
+      <c r="K22" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L22" s="39" t="s">
+      <c r="L22" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N22" s="53" t="s">
+      <c r="N22" s="51" t="s">
         <v>204</v>
       </c>
-      <c r="O22" s="39" t="s">
+      <c r="O22" s="37" t="s">
         <v>213</v>
       </c>
-      <c r="P22" s="34" t="s">
+      <c r="P22" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="R22" s="46"/>
-      <c r="S22" s="49"/>
-      <c r="T22" s="31"/>
-      <c r="U22" s="23"/>
+      <c r="R22" s="44">
+        <v>3160218</v>
+      </c>
+      <c r="S22" s="47">
+        <v>3160218</v>
+      </c>
+      <c r="T22" s="66" t="s">
+        <v>251</v>
+      </c>
+      <c r="U22" s="23" t="s">
+        <v>283</v>
+      </c>
       <c r="V22" t="s">
         <v>49</v>
       </c>
@@ -5375,7 +5789,7 @@
         <v>113</v>
       </c>
       <c r="Y22" s="1"/>
-      <c r="Z22" s="42" t="s">
+      <c r="Z22" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA22" s="20" t="s">
@@ -5384,7 +5798,7 @@
       <c r="AB22" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC22" s="42" t="s">
+      <c r="AC22" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD22" s="20" t="s">
@@ -5408,13 +5822,13 @@
       <c r="AP22" t="s">
         <v>82</v>
       </c>
-      <c r="AQ22" s="51" t="s">
+      <c r="AQ22" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR22" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS22" s="51" t="s">
+      <c r="AS22" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT22" s="1" t="s">
@@ -5470,46 +5884,54 @@
       <c r="B23" s="27">
         <v>21</v>
       </c>
-      <c r="C23" s="34" t="s">
+      <c r="C23" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D23" s="34" t="s">
+      <c r="D23" s="32" t="s">
         <v>139</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G23" s="39" t="s">
+      <c r="G23" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H23" s="39" t="s">
+      <c r="H23" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I23" s="40" t="s">
+      <c r="I23" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J23" s="39" t="s">
+      <c r="J23" s="37" t="s">
         <v>193</v>
       </c>
-      <c r="K23" s="39" t="s">
+      <c r="K23" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L23" s="39" t="s">
+      <c r="L23" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N23" s="53" t="s">
+      <c r="N23" s="51" t="s">
         <v>205</v>
       </c>
-      <c r="O23" s="39" t="s">
+      <c r="O23" s="37" t="s">
         <v>213</v>
       </c>
-      <c r="P23" s="34" t="s">
+      <c r="P23" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="R23" s="46"/>
-      <c r="S23" s="49"/>
-      <c r="T23" s="31"/>
-      <c r="U23" s="23"/>
+      <c r="R23" s="44">
+        <v>2503880</v>
+      </c>
+      <c r="S23" s="47">
+        <v>2503880</v>
+      </c>
+      <c r="T23" s="66" t="s">
+        <v>252</v>
+      </c>
+      <c r="U23" s="23" t="s">
+        <v>284</v>
+      </c>
       <c r="V23" t="s">
         <v>49</v>
       </c>
@@ -5520,7 +5942,7 @@
         <v>113</v>
       </c>
       <c r="Y23" s="1"/>
-      <c r="Z23" s="42" t="s">
+      <c r="Z23" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA23" s="20" t="s">
@@ -5529,7 +5951,7 @@
       <c r="AB23" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC23" s="42" t="s">
+      <c r="AC23" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD23" s="20" t="s">
@@ -5553,13 +5975,13 @@
       <c r="AP23" t="s">
         <v>82</v>
       </c>
-      <c r="AQ23" s="51" t="s">
+      <c r="AQ23" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR23" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS23" s="51" t="s">
+      <c r="AS23" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT23" s="1" t="s">
@@ -5615,39 +6037,39 @@
       <c r="B24" s="27">
         <v>22</v>
       </c>
-      <c r="C24" s="34" t="s">
+      <c r="C24" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="D24" s="34" t="s">
+      <c r="D24" s="32" t="s">
         <v>140</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G24" s="39" t="s">
+      <c r="G24" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H24" s="39" t="s">
+      <c r="H24" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I24" s="40" t="s">
+      <c r="I24" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J24" s="39" t="s">
+      <c r="J24" s="37" t="s">
         <v>194</v>
       </c>
-      <c r="K24" s="39" t="s">
+      <c r="K24" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L24" s="39" t="s">
+      <c r="L24" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N24" s="53" t="s">
+      <c r="N24" s="51" t="s">
         <v>206</v>
       </c>
-      <c r="R24" s="46"/>
-      <c r="S24" s="49"/>
-      <c r="T24" s="31"/>
+      <c r="R24" s="44"/>
+      <c r="S24" s="47"/>
+      <c r="T24" s="66"/>
       <c r="U24" s="23"/>
       <c r="V24" t="s">
         <v>49</v>
@@ -5659,7 +6081,7 @@
         <v>113</v>
       </c>
       <c r="Y24" s="1"/>
-      <c r="Z24" s="42" t="s">
+      <c r="Z24" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA24" s="20" t="s">
@@ -5668,7 +6090,7 @@
       <c r="AB24" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC24" s="42" t="s">
+      <c r="AC24" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD24" s="20" t="s">
@@ -5692,13 +6114,13 @@
       <c r="AP24" t="s">
         <v>82</v>
       </c>
-      <c r="AQ24" s="51" t="s">
+      <c r="AQ24" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR24" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS24" s="51" t="s">
+      <c r="AS24" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT24" s="1" t="s">
@@ -5754,46 +6176,54 @@
       <c r="B25" s="27">
         <v>23</v>
       </c>
-      <c r="C25" s="34" t="s">
+      <c r="C25" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D25" s="34" t="s">
+      <c r="D25" s="32" t="s">
         <v>141</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G25" s="39" t="s">
+      <c r="G25" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H25" s="39" t="s">
+      <c r="H25" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I25" s="40" t="s">
+      <c r="I25" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J25" s="39" t="s">
+      <c r="J25" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="K25" s="39" t="s">
+      <c r="K25" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L25" s="39" t="s">
+      <c r="L25" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N25" s="53" t="s">
+      <c r="N25" s="51" t="s">
         <v>207</v>
       </c>
-      <c r="O25" s="39" t="s">
+      <c r="O25" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="P25" s="34" t="s">
+      <c r="P25" s="32" t="s">
         <v>175</v>
       </c>
-      <c r="R25" s="46"/>
-      <c r="S25" s="49"/>
-      <c r="T25" s="31"/>
-      <c r="U25" s="23"/>
+      <c r="R25" s="44">
+        <v>2568535</v>
+      </c>
+      <c r="S25" s="47">
+        <v>2568535</v>
+      </c>
+      <c r="T25" s="66" t="s">
+        <v>253</v>
+      </c>
+      <c r="U25" s="23" t="s">
+        <v>285</v>
+      </c>
       <c r="V25" t="s">
         <v>49</v>
       </c>
@@ -5804,7 +6234,7 @@
         <v>113</v>
       </c>
       <c r="Y25" s="1"/>
-      <c r="Z25" s="42" t="s">
+      <c r="Z25" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA25" s="20" t="s">
@@ -5813,7 +6243,7 @@
       <c r="AB25" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC25" s="42" t="s">
+      <c r="AC25" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD25" s="20" t="s">
@@ -5837,13 +6267,13 @@
       <c r="AP25" t="s">
         <v>82</v>
       </c>
-      <c r="AQ25" s="51" t="s">
+      <c r="AQ25" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR25" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS25" s="51" t="s">
+      <c r="AS25" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT25" s="1" t="s">
@@ -5899,46 +6329,54 @@
       <c r="B26" s="27">
         <v>24</v>
       </c>
-      <c r="C26" s="34" t="s">
+      <c r="C26" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D26" s="34" t="s">
+      <c r="D26" s="32" t="s">
         <v>142</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G26" s="39" t="s">
+      <c r="G26" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H26" s="39" t="s">
+      <c r="H26" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I26" s="40" t="s">
+      <c r="I26" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J26" s="39" t="s">
+      <c r="J26" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="K26" s="39" t="s">
+      <c r="K26" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L26" s="39" t="s">
+      <c r="L26" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N26" s="53" t="s">
+      <c r="N26" s="51" t="s">
         <v>203</v>
       </c>
-      <c r="O26" s="39" t="s">
+      <c r="O26" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="P26" s="34" t="s">
+      <c r="P26" s="32" t="s">
         <v>175</v>
       </c>
-      <c r="R26" s="46"/>
-      <c r="S26" s="49"/>
-      <c r="T26" s="31"/>
-      <c r="U26" s="23"/>
+      <c r="R26" s="44">
+        <v>1596500</v>
+      </c>
+      <c r="S26" s="47">
+        <v>1596500</v>
+      </c>
+      <c r="T26" s="66" t="s">
+        <v>254</v>
+      </c>
+      <c r="U26" s="23" t="s">
+        <v>286</v>
+      </c>
       <c r="V26" t="s">
         <v>49</v>
       </c>
@@ -5949,7 +6387,7 @@
         <v>113</v>
       </c>
       <c r="Y26" s="1"/>
-      <c r="Z26" s="42" t="s">
+      <c r="Z26" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA26" s="20" t="s">
@@ -5958,7 +6396,7 @@
       <c r="AB26" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC26" s="42" t="s">
+      <c r="AC26" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD26" s="20" t="s">
@@ -5982,13 +6420,13 @@
       <c r="AP26" t="s">
         <v>82</v>
       </c>
-      <c r="AQ26" s="51" t="s">
+      <c r="AQ26" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR26" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS26" s="51" t="s">
+      <c r="AS26" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT26" s="1" t="s">
@@ -6044,46 +6482,54 @@
       <c r="B27" s="27">
         <v>25</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D27" s="34" t="s">
+      <c r="D27" s="32" t="s">
         <v>143</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G27" s="39" t="s">
+      <c r="G27" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H27" s="39" t="s">
+      <c r="H27" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I27" s="40" t="s">
+      <c r="I27" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J27" s="39" t="s">
+      <c r="J27" s="37" t="s">
         <v>197</v>
       </c>
-      <c r="K27" s="39" t="s">
+      <c r="K27" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L27" s="39" t="s">
+      <c r="L27" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N27" s="53" t="s">
+      <c r="N27" s="51" t="s">
         <v>204</v>
       </c>
-      <c r="O27" s="39" t="s">
+      <c r="O27" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="P27" s="34" t="s">
+      <c r="P27" s="32" t="s">
         <v>175</v>
       </c>
-      <c r="R27" s="46"/>
-      <c r="S27" s="49"/>
-      <c r="T27" s="31"/>
-      <c r="U27" s="23"/>
+      <c r="R27" s="44">
+        <v>4894294</v>
+      </c>
+      <c r="S27" s="47">
+        <v>4894294</v>
+      </c>
+      <c r="T27" s="66" t="s">
+        <v>255</v>
+      </c>
+      <c r="U27" s="23" t="s">
+        <v>287</v>
+      </c>
       <c r="V27" t="s">
         <v>49</v>
       </c>
@@ -6094,7 +6540,7 @@
         <v>113</v>
       </c>
       <c r="Y27" s="1"/>
-      <c r="Z27" s="42" t="s">
+      <c r="Z27" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA27" s="20" t="s">
@@ -6103,7 +6549,7 @@
       <c r="AB27" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC27" s="42" t="s">
+      <c r="AC27" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD27" s="20" t="s">
@@ -6127,13 +6573,13 @@
       <c r="AP27" t="s">
         <v>82</v>
       </c>
-      <c r="AQ27" s="51" t="s">
+      <c r="AQ27" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR27" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS27" s="51" t="s">
+      <c r="AS27" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT27" s="1" t="s">
@@ -6189,46 +6635,54 @@
       <c r="B28" s="27">
         <v>26</v>
       </c>
-      <c r="C28" s="34" t="s">
+      <c r="C28" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D28" s="34" t="s">
+      <c r="D28" s="32" t="s">
         <v>144</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G28" s="39" t="s">
+      <c r="G28" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H28" s="39" t="s">
+      <c r="H28" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I28" s="40" t="s">
+      <c r="I28" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J28" s="39" t="s">
+      <c r="J28" s="37" t="s">
         <v>198</v>
       </c>
-      <c r="K28" s="39" t="s">
+      <c r="K28" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L28" s="39" t="s">
+      <c r="L28" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N28" s="65" t="s">
+      <c r="N28" s="63" t="s">
         <v>206</v>
       </c>
-      <c r="O28" s="39" t="s">
+      <c r="O28" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="P28" s="34" t="s">
+      <c r="P28" s="32" t="s">
         <v>175</v>
       </c>
-      <c r="R28" s="46"/>
-      <c r="S28" s="49"/>
-      <c r="T28" s="31"/>
-      <c r="U28" s="23"/>
+      <c r="R28" s="44">
+        <v>1296196</v>
+      </c>
+      <c r="S28" s="47">
+        <v>1296196</v>
+      </c>
+      <c r="T28" s="66" t="s">
+        <v>256</v>
+      </c>
+      <c r="U28" s="23" t="s">
+        <v>288</v>
+      </c>
       <c r="V28" t="s">
         <v>49</v>
       </c>
@@ -6239,7 +6693,7 @@
         <v>113</v>
       </c>
       <c r="Y28" s="1"/>
-      <c r="Z28" s="42" t="s">
+      <c r="Z28" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA28" s="20" t="s">
@@ -6248,7 +6702,7 @@
       <c r="AB28" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC28" s="42" t="s">
+      <c r="AC28" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD28" s="20" t="s">
@@ -6272,13 +6726,13 @@
       <c r="AP28" t="s">
         <v>82</v>
       </c>
-      <c r="AQ28" s="51" t="s">
+      <c r="AQ28" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR28" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS28" s="51" t="s">
+      <c r="AS28" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT28" s="1" t="s">
@@ -6334,46 +6788,54 @@
       <c r="B29" s="27">
         <v>27</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="C29" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D29" s="34" t="s">
+      <c r="D29" s="32" t="s">
         <v>145</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G29" s="39" t="s">
+      <c r="G29" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H29" s="39" t="s">
+      <c r="H29" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I29" s="40" t="s">
+      <c r="I29" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J29" s="39" t="s">
+      <c r="J29" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="K29" s="39" t="s">
+      <c r="K29" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L29" s="39" t="s">
+      <c r="L29" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N29" s="53" t="s">
+      <c r="N29" s="51" t="s">
         <v>206</v>
       </c>
-      <c r="O29" s="39" t="s">
+      <c r="O29" s="37" t="s">
         <v>215</v>
       </c>
-      <c r="P29" s="34" t="s">
+      <c r="P29" s="32" t="s">
         <v>176</v>
       </c>
-      <c r="R29" s="46"/>
-      <c r="S29" s="49"/>
-      <c r="T29" s="31"/>
-      <c r="U29" s="23"/>
+      <c r="R29" s="44">
+        <v>1549054</v>
+      </c>
+      <c r="S29" s="47">
+        <v>1549054</v>
+      </c>
+      <c r="T29" s="66" t="s">
+        <v>257</v>
+      </c>
+      <c r="U29" s="23" t="s">
+        <v>289</v>
+      </c>
       <c r="V29" t="s">
         <v>49</v>
       </c>
@@ -6384,7 +6846,7 @@
         <v>114</v>
       </c>
       <c r="Y29" s="1"/>
-      <c r="Z29" s="42" t="s">
+      <c r="Z29" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA29" s="20" t="s">
@@ -6393,7 +6855,7 @@
       <c r="AB29" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC29" s="42" t="s">
+      <c r="AC29" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD29" s="20" t="s">
@@ -6417,13 +6879,13 @@
       <c r="AP29" t="s">
         <v>82</v>
       </c>
-      <c r="AQ29" s="51" t="s">
+      <c r="AQ29" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR29" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS29" s="51" t="s">
+      <c r="AS29" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT29" s="1" t="s">
@@ -6479,46 +6941,54 @@
       <c r="B30" s="27">
         <v>28</v>
       </c>
-      <c r="C30" s="34" t="s">
+      <c r="C30" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D30" s="34" t="s">
+      <c r="D30" s="32" t="s">
         <v>146</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G30" s="39" t="s">
+      <c r="G30" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H30" s="39" t="s">
+      <c r="H30" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I30" s="40" t="s">
+      <c r="I30" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J30" s="39" t="s">
+      <c r="J30" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="K30" s="39" t="s">
+      <c r="K30" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L30" s="39" t="s">
+      <c r="L30" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N30" s="53" t="s">
+      <c r="N30" s="51" t="s">
         <v>203</v>
       </c>
-      <c r="O30" s="39" t="s">
+      <c r="O30" s="37" t="s">
         <v>215</v>
       </c>
-      <c r="P30" s="34" t="s">
+      <c r="P30" s="32" t="s">
         <v>176</v>
       </c>
-      <c r="R30" s="46"/>
-      <c r="S30" s="49"/>
-      <c r="T30" s="31"/>
-      <c r="U30" s="23"/>
+      <c r="R30" s="44">
+        <v>115903</v>
+      </c>
+      <c r="S30" s="47">
+        <v>115903</v>
+      </c>
+      <c r="T30" s="66" t="s">
+        <v>258</v>
+      </c>
+      <c r="U30" s="23" t="s">
+        <v>290</v>
+      </c>
       <c r="V30" t="s">
         <v>49</v>
       </c>
@@ -6529,7 +6999,7 @@
         <v>115</v>
       </c>
       <c r="Y30" s="1"/>
-      <c r="Z30" s="42" t="s">
+      <c r="Z30" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA30" s="20" t="s">
@@ -6538,7 +7008,7 @@
       <c r="AB30" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC30" s="42" t="s">
+      <c r="AC30" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD30" s="20" t="s">
@@ -6562,13 +7032,13 @@
       <c r="AP30" t="s">
         <v>82</v>
       </c>
-      <c r="AQ30" s="51" t="s">
+      <c r="AQ30" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR30" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS30" s="51" t="s">
+      <c r="AS30" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT30" s="1" t="s">
@@ -6624,46 +7094,54 @@
       <c r="B31" s="27">
         <v>29</v>
       </c>
-      <c r="C31" s="34" t="s">
+      <c r="C31" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D31" s="34" t="s">
+      <c r="D31" s="32" t="s">
         <v>147</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G31" s="39" t="s">
+      <c r="G31" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H31" s="39" t="s">
+      <c r="H31" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I31" s="40" t="s">
+      <c r="I31" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J31" s="39" t="s">
+      <c r="J31" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="K31" s="39" t="s">
+      <c r="K31" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L31" s="39" t="s">
+      <c r="L31" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N31" s="53" t="s">
+      <c r="N31" s="51" t="s">
         <v>204</v>
       </c>
-      <c r="O31" s="39" t="s">
+      <c r="O31" s="37" t="s">
         <v>215</v>
       </c>
-      <c r="P31" s="34" t="s">
+      <c r="P31" s="32" t="s">
         <v>176</v>
       </c>
-      <c r="R31" s="46"/>
-      <c r="S31" s="49"/>
-      <c r="T31" s="31"/>
-      <c r="U31" s="23"/>
+      <c r="R31" s="44">
+        <v>2854812</v>
+      </c>
+      <c r="S31" s="47">
+        <v>2854812</v>
+      </c>
+      <c r="T31" s="66" t="s">
+        <v>259</v>
+      </c>
+      <c r="U31" s="23" t="s">
+        <v>291</v>
+      </c>
       <c r="V31" t="s">
         <v>49</v>
       </c>
@@ -6674,7 +7152,7 @@
         <v>115</v>
       </c>
       <c r="Y31" s="1"/>
-      <c r="Z31" s="42" t="s">
+      <c r="Z31" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA31" s="20" t="s">
@@ -6683,7 +7161,7 @@
       <c r="AB31" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC31" s="42" t="s">
+      <c r="AC31" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD31" s="20" t="s">
@@ -6707,13 +7185,13 @@
       <c r="AP31" t="s">
         <v>82</v>
       </c>
-      <c r="AQ31" s="51" t="s">
+      <c r="AQ31" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR31" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS31" s="51" t="s">
+      <c r="AS31" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT31" s="1" t="s">
@@ -6769,46 +7247,54 @@
       <c r="B32" s="27">
         <v>30</v>
       </c>
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D32" s="34" t="s">
+      <c r="D32" s="32" t="s">
         <v>148</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G32" s="39" t="s">
+      <c r="G32" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H32" s="39" t="s">
+      <c r="H32" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I32" s="40" t="s">
+      <c r="I32" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J32" s="39" t="s">
+      <c r="J32" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="K32" s="39" t="s">
+      <c r="K32" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L32" s="39" t="s">
+      <c r="L32" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N32" s="53" t="s">
+      <c r="N32" s="51" t="s">
         <v>205</v>
       </c>
-      <c r="O32" s="39" t="s">
+      <c r="O32" s="37" t="s">
         <v>215</v>
       </c>
-      <c r="P32" s="34" t="s">
+      <c r="P32" s="32" t="s">
         <v>176</v>
       </c>
-      <c r="R32" s="46"/>
-      <c r="S32" s="49"/>
-      <c r="T32" s="31"/>
-      <c r="U32" s="23"/>
+      <c r="R32" s="44">
+        <v>1989636</v>
+      </c>
+      <c r="S32" s="47">
+        <v>1989636</v>
+      </c>
+      <c r="T32" s="66" t="s">
+        <v>260</v>
+      </c>
+      <c r="U32" s="23" t="s">
+        <v>292</v>
+      </c>
       <c r="V32" t="s">
         <v>49</v>
       </c>
@@ -6819,7 +7305,7 @@
         <v>115</v>
       </c>
       <c r="Y32" s="1"/>
-      <c r="Z32" s="42" t="s">
+      <c r="Z32" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA32" s="20" t="s">
@@ -6828,7 +7314,7 @@
       <c r="AB32" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC32" s="42" t="s">
+      <c r="AC32" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD32" s="20" t="s">
@@ -6852,13 +7338,13 @@
       <c r="AP32" t="s">
         <v>82</v>
       </c>
-      <c r="AQ32" s="51" t="s">
+      <c r="AQ32" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR32" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS32" s="51" t="s">
+      <c r="AS32" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT32" s="1" t="s">
@@ -6914,46 +7400,54 @@
       <c r="B33" s="27">
         <v>31</v>
       </c>
-      <c r="C33" s="34" t="s">
+      <c r="C33" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D33" s="34" t="s">
+      <c r="D33" s="32" t="s">
         <v>149</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G33" s="39" t="s">
+      <c r="G33" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H33" s="39" t="s">
+      <c r="H33" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I33" s="40" t="s">
+      <c r="I33" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J33" s="39" t="s">
+      <c r="J33" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="K33" s="39" t="s">
+      <c r="K33" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L33" s="39" t="s">
+      <c r="L33" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N33" s="53" t="s">
+      <c r="N33" s="51" t="s">
         <v>204</v>
       </c>
-      <c r="O33" s="39" t="s">
+      <c r="O33" s="37" t="s">
         <v>216</v>
       </c>
-      <c r="P33" s="34" t="s">
+      <c r="P33" s="32" t="s">
         <v>177</v>
       </c>
-      <c r="R33" s="46"/>
-      <c r="S33" s="49"/>
-      <c r="T33" s="32"/>
-      <c r="U33" s="23"/>
+      <c r="R33" s="44">
+        <v>1449582</v>
+      </c>
+      <c r="S33" s="47">
+        <v>1449582</v>
+      </c>
+      <c r="T33" s="66" t="s">
+        <v>261</v>
+      </c>
+      <c r="U33" s="23" t="s">
+        <v>293</v>
+      </c>
       <c r="V33" t="s">
         <v>49</v>
       </c>
@@ -6964,7 +7458,7 @@
         <v>115</v>
       </c>
       <c r="Y33" s="1"/>
-      <c r="Z33" s="42" t="s">
+      <c r="Z33" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA33" s="20" t="s">
@@ -6973,7 +7467,7 @@
       <c r="AB33" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC33" s="42" t="s">
+      <c r="AC33" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD33" s="20" t="s">
@@ -6997,13 +7491,13 @@
       <c r="AP33" t="s">
         <v>82</v>
       </c>
-      <c r="AQ33" s="51" t="s">
+      <c r="AQ33" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR33" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS33" s="51" t="s">
+      <c r="AS33" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT33" s="1" t="s">
@@ -7059,46 +7553,54 @@
       <c r="B34" s="27">
         <v>32</v>
       </c>
-      <c r="C34" s="34" t="s">
+      <c r="C34" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D34" s="34" t="s">
+      <c r="D34" s="32" t="s">
         <v>150</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G34" s="39" t="s">
+      <c r="G34" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H34" s="39" t="s">
+      <c r="H34" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I34" s="40" t="s">
+      <c r="I34" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J34" s="39" t="s">
+      <c r="J34" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="K34" s="39" t="s">
+      <c r="K34" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L34" s="39" t="s">
+      <c r="L34" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N34" s="53" t="s">
+      <c r="N34" s="51" t="s">
         <v>205</v>
       </c>
-      <c r="O34" s="39" t="s">
+      <c r="O34" s="37" t="s">
         <v>216</v>
       </c>
-      <c r="P34" s="34" t="s">
+      <c r="P34" s="32" t="s">
         <v>177</v>
       </c>
-      <c r="R34" s="46"/>
-      <c r="S34" s="49"/>
-      <c r="T34" s="31"/>
-      <c r="U34" s="23"/>
+      <c r="R34" s="44">
+        <v>1273971</v>
+      </c>
+      <c r="S34" s="47">
+        <v>1273971</v>
+      </c>
+      <c r="T34" s="67" t="s">
+        <v>262</v>
+      </c>
+      <c r="U34" s="23" t="s">
+        <v>294</v>
+      </c>
       <c r="V34" t="s">
         <v>49</v>
       </c>
@@ -7109,7 +7611,7 @@
         <v>115</v>
       </c>
       <c r="Y34" s="1"/>
-      <c r="Z34" s="42" t="s">
+      <c r="Z34" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA34" s="20" t="s">
@@ -7118,7 +7620,7 @@
       <c r="AB34" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC34" s="42" t="s">
+      <c r="AC34" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD34" s="20" t="s">
@@ -7142,13 +7644,13 @@
       <c r="AP34" t="s">
         <v>82</v>
       </c>
-      <c r="AQ34" s="51" t="s">
+      <c r="AQ34" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR34" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS34" s="51" t="s">
+      <c r="AS34" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT34" s="1" t="s">
@@ -7197,49 +7699,64 @@
       <c r="CB34"/>
     </row>
     <row r="35" spans="1:80" x14ac:dyDescent="0.2">
-      <c r="A35" s="67">
+      <c r="A35" s="64">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B35" s="27">
         <v>33</v>
       </c>
-      <c r="C35" s="34" t="s">
+      <c r="C35" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D35" s="34" t="s">
+      <c r="D35" s="32" t="s">
         <v>222</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="F35" s="36"/>
-      <c r="G35" s="39" t="s">
+      <c r="F35" s="34"/>
+      <c r="G35" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="H35" s="39" t="s">
+      <c r="H35" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="I35" s="40" t="s">
+      <c r="I35" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="J35" s="39" t="s">
+      <c r="J35" s="37" t="s">
         <v>224</v>
       </c>
-      <c r="K35" s="39" t="s">
+      <c r="K35" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="L35" s="39" t="s">
+      <c r="L35" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="N35" s="53" t="s">
+      <c r="N35" s="51" t="s">
         <v>206</v>
       </c>
-      <c r="O35" s="39" t="s">
+      <c r="O35" s="37" t="s">
         <v>216</v>
       </c>
-      <c r="P35" s="34" t="s">
+      <c r="P35" s="32" t="s">
         <v>177</v>
+      </c>
+      <c r="R35" s="44">
+        <v>3767045</v>
+      </c>
+      <c r="S35" s="47">
+        <v>3767045</v>
+      </c>
+      <c r="T35" s="66" t="s">
+        <v>263</v>
+      </c>
+      <c r="U35" s="23" t="s">
+        <v>295</v>
+      </c>
+      <c r="V35" t="s">
+        <v>49</v>
       </c>
       <c r="W35" s="20" t="s">
         <v>225</v>
@@ -7247,7 +7764,7 @@
       <c r="X35" s="20" t="s">
         <v>226</v>
       </c>
-      <c r="Z35" s="42" t="s">
+      <c r="Z35" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA35" s="20" t="s">
@@ -7256,7 +7773,7 @@
       <c r="AB35" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AC35" s="42" t="s">
+      <c r="AC35" s="40" t="s">
         <v>75</v>
       </c>
       <c r="AD35" s="20" t="s">
@@ -7275,13 +7792,13 @@
       <c r="AP35" t="s">
         <v>82</v>
       </c>
-      <c r="AQ35" s="51" t="s">
+      <c r="AQ35" s="49" t="s">
         <v>78</v>
       </c>
       <c r="AR35" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS35" s="51" t="s">
+      <c r="AS35" s="49" t="s">
         <v>77</v>
       </c>
       <c r="AT35" s="1" t="s">
@@ -7328,8 +7845,9 @@
     <row r="36" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A36"/>
       <c r="E36"/>
-      <c r="F36" s="36"/>
-      <c r="I36" s="39"/>
+      <c r="F36" s="34"/>
+      <c r="I36" s="37"/>
+      <c r="T36" s="2"/>
       <c r="W36"/>
       <c r="X36"/>
       <c r="Z36" s="2"/>
@@ -7360,6 +7878,7 @@
       <c r="CB36"/>
     </row>
     <row r="37" spans="1:80" x14ac:dyDescent="0.2">
+      <c r="T37" s="2"/>
       <c r="AN37" s="15"/>
     </row>
     <row r="38" spans="1:80" x14ac:dyDescent="0.2">
@@ -7448,19 +7967,9 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
-      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
-      <rowBreaks count="2" manualBreakCount="2">
-        <brk id="1" max="16383" man="1"/>
-        <brk id="325" max="16383" man="1"/>
-      </rowBreaks>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
-      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
+    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
+      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
@@ -7478,14 +7987,24 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
-      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
+    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
+      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
       </rowBreaks>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
+      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
+      <rowBreaks count="2" manualBreakCount="2">
+        <brk id="1" max="16383" man="1"/>
+        <brk id="325" max="16383" man="1"/>
+      </rowBreaks>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -7496,10 +8015,10 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="AM3:AM34">
-    <cfRule type="containsBlanks" dxfId="4" priority="9" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="10" priority="9" stopIfTrue="1">
       <formula>LEN(TRIM(AM3))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="lessThan">
       <formula>0.02</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7512,16 +8031,16 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R3:S34">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="lessThan">
+  <conditionalFormatting sqref="R3:S35">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="lessThan">
       <formula>2000</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7">
+    <cfRule type="expression" dxfId="7" priority="7">
       <formula>$R3&lt;&gt;$S3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2:S34 R37:S1048576">
-    <cfRule type="containsBlanks" dxfId="0" priority="1" stopIfTrue="1">
+  <conditionalFormatting sqref="R37:S1048576 R2:S35">
+    <cfRule type="containsBlanks" dxfId="6" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(R2))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added read counts and md5 check sums
</commit_message>
<xml_diff>
--- a/metadata/excel/projects/micans/micans_v6_exp1/metadata.xlsx
+++ b/metadata/excel/projects/micans/micans_v6_exp1/metadata.xlsx
@@ -16,10 +16,10 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="LS - Personal View" guid="{06B92370-743D-804F-912C-658BE37B1274}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
     <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="LS - Personal View" guid="{06B92370-743D-804F-912C-658BE37B1274}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -1673,14 +1673,14 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="11" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="290">
@@ -1975,69 +1975,7 @@
     <cellStyle name="Hyperlink" xfId="288" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color auto="1"/>
@@ -2568,24 +2506,24 @@
       <c r="BB1" s="5"/>
       <c r="BC1" s="5"/>
       <c r="BD1" s="12"/>
-      <c r="BF1" s="65" t="s">
+      <c r="BF1" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="BG1" s="65"/>
-      <c r="BH1" s="65"/>
-      <c r="BI1" s="65"/>
-      <c r="BK1" s="65" t="s">
+      <c r="BG1" s="67"/>
+      <c r="BH1" s="67"/>
+      <c r="BI1" s="67"/>
+      <c r="BK1" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="BL1" s="65"/>
-      <c r="BM1" s="65"/>
-      <c r="BN1" s="65"/>
-      <c r="BO1" s="65"/>
-      <c r="BP1" s="65"/>
-      <c r="BR1" s="65" t="s">
+      <c r="BL1" s="67"/>
+      <c r="BM1" s="67"/>
+      <c r="BN1" s="67"/>
+      <c r="BO1" s="67"/>
+      <c r="BP1" s="67"/>
+      <c r="BR1" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="BS1" s="65"/>
+      <c r="BS1" s="67"/>
       <c r="BU1" s="10" t="s">
         <v>72</v>
       </c>
@@ -2866,7 +2804,7 @@
       <c r="S3" s="47">
         <v>2820243</v>
       </c>
-      <c r="T3" s="66" t="s">
+      <c r="T3" s="65" t="s">
         <v>232</v>
       </c>
       <c r="U3" s="23" t="s">
@@ -3019,7 +2957,7 @@
       <c r="S4" s="47">
         <v>1695054</v>
       </c>
-      <c r="T4" s="66" t="s">
+      <c r="T4" s="65" t="s">
         <v>233</v>
       </c>
       <c r="U4" s="23" t="s">
@@ -3172,7 +3110,7 @@
       <c r="S5" s="47">
         <v>1471424</v>
       </c>
-      <c r="T5" s="66" t="s">
+      <c r="T5" s="65" t="s">
         <v>234</v>
       </c>
       <c r="U5" s="28" t="s">
@@ -3325,7 +3263,7 @@
       <c r="S6" s="47">
         <v>1189163</v>
       </c>
-      <c r="T6" s="67" t="s">
+      <c r="T6" s="66" t="s">
         <v>235</v>
       </c>
       <c r="U6" s="23" t="s">
@@ -3478,7 +3416,7 @@
       <c r="S7" s="47">
         <v>1518563</v>
       </c>
-      <c r="T7" s="66" t="s">
+      <c r="T7" s="65" t="s">
         <v>236</v>
       </c>
       <c r="U7" s="23" t="s">
@@ -3631,7 +3569,7 @@
       <c r="S8" s="47">
         <v>1992368</v>
       </c>
-      <c r="T8" s="66" t="s">
+      <c r="T8" s="65" t="s">
         <v>237</v>
       </c>
       <c r="U8" s="28" t="s">
@@ -3784,7 +3722,7 @@
       <c r="S9" s="47">
         <v>778194</v>
       </c>
-      <c r="T9" s="66" t="s">
+      <c r="T9" s="65" t="s">
         <v>238</v>
       </c>
       <c r="U9" s="23" t="s">
@@ -3937,7 +3875,7 @@
       <c r="S10" s="47">
         <v>2162643</v>
       </c>
-      <c r="T10" s="66" t="s">
+      <c r="T10" s="65" t="s">
         <v>239</v>
       </c>
       <c r="U10" s="23" t="s">
@@ -4090,7 +4028,7 @@
       <c r="S11" s="47">
         <v>550318</v>
       </c>
-      <c r="T11" s="66" t="s">
+      <c r="T11" s="65" t="s">
         <v>240</v>
       </c>
       <c r="U11" s="23" t="s">
@@ -4243,7 +4181,7 @@
       <c r="S12" s="47">
         <v>1673873</v>
       </c>
-      <c r="T12" s="66" t="s">
+      <c r="T12" s="65" t="s">
         <v>241</v>
       </c>
       <c r="U12" s="28" t="s">
@@ -4396,7 +4334,7 @@
       <c r="S13" s="47">
         <v>1249513</v>
       </c>
-      <c r="T13" s="66" t="s">
+      <c r="T13" s="65" t="s">
         <v>242</v>
       </c>
       <c r="U13" s="23" t="s">
@@ -4549,7 +4487,7 @@
       <c r="S14" s="47">
         <v>629046</v>
       </c>
-      <c r="T14" s="66" t="s">
+      <c r="T14" s="65" t="s">
         <v>243</v>
       </c>
       <c r="U14" s="23" t="s">
@@ -4702,7 +4640,7 @@
       <c r="S15" s="47">
         <v>96651</v>
       </c>
-      <c r="T15" s="66" t="s">
+      <c r="T15" s="65" t="s">
         <v>244</v>
       </c>
       <c r="U15" s="23" t="s">
@@ -4855,7 +4793,7 @@
       <c r="S16" s="47">
         <v>173299</v>
       </c>
-      <c r="T16" s="66" t="s">
+      <c r="T16" s="65" t="s">
         <v>245</v>
       </c>
       <c r="U16" s="23" t="s">
@@ -5008,7 +4946,7 @@
       <c r="S17" s="47">
         <v>1867219</v>
       </c>
-      <c r="T17" s="67" t="s">
+      <c r="T17" s="66" t="s">
         <v>246</v>
       </c>
       <c r="U17" s="23" t="s">
@@ -5161,7 +5099,7 @@
       <c r="S18" s="47">
         <v>1495186</v>
       </c>
-      <c r="T18" s="66" t="s">
+      <c r="T18" s="65" t="s">
         <v>247</v>
       </c>
       <c r="U18" s="23" t="s">
@@ -5314,7 +5252,7 @@
       <c r="S19" s="47">
         <v>1807248</v>
       </c>
-      <c r="T19" s="66" t="s">
+      <c r="T19" s="65" t="s">
         <v>248</v>
       </c>
       <c r="U19" s="23" t="s">
@@ -5467,7 +5405,7 @@
       <c r="S20" s="47">
         <v>1408298</v>
       </c>
-      <c r="T20" s="66" t="s">
+      <c r="T20" s="65" t="s">
         <v>249</v>
       </c>
       <c r="U20" s="23" t="s">
@@ -5620,7 +5558,7 @@
       <c r="S21" s="47">
         <v>3202907</v>
       </c>
-      <c r="T21" s="66" t="s">
+      <c r="T21" s="65" t="s">
         <v>250</v>
       </c>
       <c r="U21" s="23" t="s">
@@ -5773,7 +5711,7 @@
       <c r="S22" s="47">
         <v>3160218</v>
       </c>
-      <c r="T22" s="66" t="s">
+      <c r="T22" s="65" t="s">
         <v>251</v>
       </c>
       <c r="U22" s="23" t="s">
@@ -5926,7 +5864,7 @@
       <c r="S23" s="47">
         <v>2503880</v>
       </c>
-      <c r="T23" s="66" t="s">
+      <c r="T23" s="65" t="s">
         <v>252</v>
       </c>
       <c r="U23" s="23" t="s">
@@ -6069,7 +6007,7 @@
       </c>
       <c r="R24" s="44"/>
       <c r="S24" s="47"/>
-      <c r="T24" s="66"/>
+      <c r="T24" s="65"/>
       <c r="U24" s="23"/>
       <c r="V24" t="s">
         <v>49</v>
@@ -6218,7 +6156,7 @@
       <c r="S25" s="47">
         <v>2568535</v>
       </c>
-      <c r="T25" s="66" t="s">
+      <c r="T25" s="65" t="s">
         <v>253</v>
       </c>
       <c r="U25" s="23" t="s">
@@ -6371,7 +6309,7 @@
       <c r="S26" s="47">
         <v>1596500</v>
       </c>
-      <c r="T26" s="66" t="s">
+      <c r="T26" s="65" t="s">
         <v>254</v>
       </c>
       <c r="U26" s="23" t="s">
@@ -6524,7 +6462,7 @@
       <c r="S27" s="47">
         <v>4894294</v>
       </c>
-      <c r="T27" s="66" t="s">
+      <c r="T27" s="65" t="s">
         <v>255</v>
       </c>
       <c r="U27" s="23" t="s">
@@ -6677,7 +6615,7 @@
       <c r="S28" s="47">
         <v>1296196</v>
       </c>
-      <c r="T28" s="66" t="s">
+      <c r="T28" s="65" t="s">
         <v>256</v>
       </c>
       <c r="U28" s="23" t="s">
@@ -6830,7 +6768,7 @@
       <c r="S29" s="47">
         <v>1549054</v>
       </c>
-      <c r="T29" s="66" t="s">
+      <c r="T29" s="65" t="s">
         <v>257</v>
       </c>
       <c r="U29" s="23" t="s">
@@ -6983,7 +6921,7 @@
       <c r="S30" s="47">
         <v>115903</v>
       </c>
-      <c r="T30" s="66" t="s">
+      <c r="T30" s="65" t="s">
         <v>258</v>
       </c>
       <c r="U30" s="23" t="s">
@@ -7136,7 +7074,7 @@
       <c r="S31" s="47">
         <v>2854812</v>
       </c>
-      <c r="T31" s="66" t="s">
+      <c r="T31" s="65" t="s">
         <v>259</v>
       </c>
       <c r="U31" s="23" t="s">
@@ -7289,7 +7227,7 @@
       <c r="S32" s="47">
         <v>1989636</v>
       </c>
-      <c r="T32" s="66" t="s">
+      <c r="T32" s="65" t="s">
         <v>260</v>
       </c>
       <c r="U32" s="23" t="s">
@@ -7442,7 +7380,7 @@
       <c r="S33" s="47">
         <v>1449582</v>
       </c>
-      <c r="T33" s="66" t="s">
+      <c r="T33" s="65" t="s">
         <v>261</v>
       </c>
       <c r="U33" s="23" t="s">
@@ -7595,7 +7533,7 @@
       <c r="S34" s="47">
         <v>1273971</v>
       </c>
-      <c r="T34" s="67" t="s">
+      <c r="T34" s="66" t="s">
         <v>262</v>
       </c>
       <c r="U34" s="23" t="s">
@@ -7749,7 +7687,7 @@
       <c r="S35" s="47">
         <v>3767045</v>
       </c>
-      <c r="T35" s="66" t="s">
+      <c r="T35" s="65" t="s">
         <v>263</v>
       </c>
       <c r="U35" s="23" t="s">
@@ -7967,9 +7905,19 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
-      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
+    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
+      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
+      <rowBreaks count="2" manualBreakCount="2">
+        <brk id="1" max="16383" man="1"/>
+        <brk id="325" max="16383" man="1"/>
+      </rowBreaks>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
+      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
@@ -7987,24 +7935,14 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
-      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
+    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
+      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
       </rowBreaks>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
-      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
-      <rowBreaks count="2" manualBreakCount="2">
-        <brk id="1" max="16383" man="1"/>
-        <brk id="325" max="16383" man="1"/>
-      </rowBreaks>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -8015,10 +7953,10 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="AM3:AM34">
-    <cfRule type="containsBlanks" dxfId="10" priority="9" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="4" priority="9" stopIfTrue="1">
       <formula>LEN(TRIM(AM3))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="10" operator="lessThan">
       <formula>0.02</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8032,15 +7970,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3:S35">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="lessThan">
       <formula>2000</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="1" priority="7">
       <formula>$R3&lt;&gt;$S3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R37:S1048576 R2:S35">
-    <cfRule type="containsBlanks" dxfId="6" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(R2))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>